<commit_message>
se usan apis de crossref y openalex
</commit_message>
<xml_diff>
--- a/referencias_con_topicos.xlsx
+++ b/referencias_con_topicos.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I178"/>
+  <dimension ref="A1:I175"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -505,14 +505,14 @@
         </is>
       </c>
       <c r="F2" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="G2" t="n">
-        <v>0.588964581489563</v>
+        <v>0.6247495412826538</v>
       </c>
       <c r="H2" t="inlineStr">
         <is>
-          <t>Tópico 2: protein, effector, sequence</t>
+          <t>Tópico 3: protein, effector, sequence</t>
         </is>
       </c>
       <c r="I2" t="inlineStr">
@@ -549,11 +549,11 @@
         <v>2</v>
       </c>
       <c r="G3" t="n">
-        <v>0.3136168122291565</v>
+        <v>0.7487729787826538</v>
       </c>
       <c r="H3" t="inlineStr">
         <is>
-          <t>Tópico 3: nitrogen, model, soil</t>
+          <t>Tópico 3: protein, effector, sequence</t>
         </is>
       </c>
       <c r="I3" t="inlineStr">
@@ -587,14 +587,14 @@
         </is>
       </c>
       <c r="F4" t="n">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="G4" t="n">
-        <v>0.993877649307251</v>
+        <v>0.9131021499633789</v>
       </c>
       <c r="H4" t="inlineStr">
         <is>
-          <t>Tópico 1: model, nitrogen, network</t>
+          <t>Tópico 5: crop, soil, system</t>
         </is>
       </c>
       <c r="I4" t="inlineStr">
@@ -628,14 +628,14 @@
         </is>
       </c>
       <c r="F5" t="n">
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="G5" t="n">
-        <v>0.8505737781524658</v>
+        <v>0.6868104338645935</v>
       </c>
       <c r="H5" t="inlineStr">
         <is>
-          <t>Tópico 6: cassava, accuracy, feature</t>
+          <t>Tópico 1: cassava, blight, potato</t>
         </is>
       </c>
       <c r="I5" t="inlineStr">
@@ -669,14 +669,14 @@
         </is>
       </c>
       <c r="F6" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="G6" t="n">
-        <v>0.9938790798187256</v>
+        <v>0.784515380859375</v>
       </c>
       <c r="H6" t="inlineStr">
         <is>
-          <t>Tópico 1: model, nitrogen, network</t>
+          <t>Tópico 3: protein, effector, sequence</t>
         </is>
       </c>
       <c r="I6" t="inlineStr">
@@ -710,14 +710,14 @@
         </is>
       </c>
       <c r="F7" t="n">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="G7" t="n">
-        <v>0.6203692555427551</v>
+        <v>0.7867923378944397</v>
       </c>
       <c r="H7" t="inlineStr">
         <is>
-          <t>Tópico 5: protein, approach, performance</t>
+          <t>Tópico 3: protein, effector, sequence</t>
         </is>
       </c>
       <c r="I7" t="inlineStr">
@@ -751,14 +751,14 @@
         </is>
       </c>
       <c r="F8" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="G8" t="n">
-        <v>0.4059958755970001</v>
+        <v>0.5940303802490234</v>
       </c>
       <c r="H8" t="inlineStr">
         <is>
-          <t>Tópico 6: cassava, accuracy, feature</t>
+          <t>Tópico 5: crop, soil, system</t>
         </is>
       </c>
       <c r="I8" t="inlineStr">
@@ -792,14 +792,14 @@
         </is>
       </c>
       <c r="F9" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="G9" t="n">
-        <v>0.7659521102905273</v>
+        <v>0.5551313757896423</v>
       </c>
       <c r="H9" t="inlineStr">
         <is>
-          <t>Tópico 4: gene, bacterial, target</t>
+          <t>Tópico 3: protein, effector, sequence</t>
         </is>
       </c>
       <c r="I9" t="inlineStr">
@@ -833,14 +833,14 @@
         </is>
       </c>
       <c r="F10" t="n">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="G10" t="n">
-        <v>0.6350106596946716</v>
+        <v>0.4917862117290497</v>
       </c>
       <c r="H10" t="inlineStr">
         <is>
-          <t>Tópico 6: cassava, accuracy, feature</t>
+          <t>Tópico 7: model, data, study</t>
         </is>
       </c>
       <c r="I10" t="inlineStr">
@@ -874,14 +874,14 @@
         </is>
       </c>
       <c r="F11" t="n">
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="G11" t="n">
-        <v>0.4280872941017151</v>
+        <v>0.7995083928108215</v>
       </c>
       <c r="H11" t="inlineStr">
         <is>
-          <t>Tópico 8: crop, soil, tomato</t>
+          <t>Tópico 4: yolov, increase, map</t>
         </is>
       </c>
       <c r="I11" t="inlineStr">
@@ -915,14 +915,14 @@
         </is>
       </c>
       <c r="F12" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="G12" t="n">
-        <v>0.9086236357688904</v>
+        <v>0.5769309401512146</v>
       </c>
       <c r="H12" t="inlineStr">
         <is>
-          <t>Tópico 2: protein, effector, sequence</t>
+          <t>Tópico 3: protein, effector, sequence</t>
         </is>
       </c>
       <c r="I12" t="inlineStr">
@@ -956,14 +956,14 @@
         </is>
       </c>
       <c r="F13" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="G13" t="n">
-        <v>0.6934852004051208</v>
+        <v>0.8011610507965088</v>
       </c>
       <c r="H13" t="inlineStr">
         <is>
-          <t>Tópico 6: cassava, accuracy, feature</t>
+          <t>Tópico 5: crop, soil, system</t>
         </is>
       </c>
       <c r="I13" t="inlineStr">
@@ -997,14 +997,14 @@
         </is>
       </c>
       <c r="F14" t="n">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="G14" t="n">
-        <v>0.5011571049690247</v>
+        <v>0.9924077391624451</v>
       </c>
       <c r="H14" t="inlineStr">
         <is>
-          <t>Tópico 5: protein, approach, performance</t>
+          <t>Tópico 3: protein, effector, sequence</t>
         </is>
       </c>
       <c r="I14" t="inlineStr">
@@ -1038,14 +1038,14 @@
         </is>
       </c>
       <c r="F15" t="n">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="G15" t="n">
-        <v>0.7465940713882446</v>
+        <v>0.3629493415355682</v>
       </c>
       <c r="H15" t="inlineStr">
         <is>
-          <t>Tópico 3: nitrogen, model, soil</t>
+          <t>Tópico 5: crop, soil, system</t>
         </is>
       </c>
       <c r="I15" t="inlineStr">
@@ -1079,14 +1079,14 @@
         </is>
       </c>
       <c r="F16" t="n">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="G16" t="n">
-        <v>0.5444998145103455</v>
+        <v>0.7002357244491577</v>
       </c>
       <c r="H16" t="inlineStr">
         <is>
-          <t>Tópico 5: protein, approach, performance</t>
+          <t>Tópico 3: protein, effector, sequence</t>
         </is>
       </c>
       <c r="I16" t="inlineStr">
@@ -1120,14 +1120,14 @@
         </is>
       </c>
       <c r="F17" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="G17" t="n">
-        <v>0.9950485229492188</v>
+        <v>0.9947812557220459</v>
       </c>
       <c r="H17" t="inlineStr">
         <is>
-          <t>Tópico 2: protein, effector, sequence</t>
+          <t>Tópico 3: protein, effector, sequence</t>
         </is>
       </c>
       <c r="I17" t="inlineStr">
@@ -1161,14 +1161,14 @@
         </is>
       </c>
       <c r="F18" t="n">
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="G18" t="n">
-        <v>0.9947980642318726</v>
+        <v>0.3722582757472992</v>
       </c>
       <c r="H18" t="inlineStr">
         <is>
-          <t>Tópico 6: cassava, accuracy, feature</t>
+          <t>Tópico 1: cassava, blight, potato</t>
         </is>
       </c>
       <c r="I18" t="inlineStr">
@@ -1202,14 +1202,14 @@
         </is>
       </c>
       <c r="F19" t="n">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="G19" t="n">
-        <v>0.9875849485397339</v>
+        <v>0.5466776490211487</v>
       </c>
       <c r="H19" t="inlineStr">
         <is>
-          <t>Tópico 5: protein, approach, performance</t>
+          <t>Tópico 3: protein, effector, sequence</t>
         </is>
       </c>
       <c r="I19" t="inlineStr">
@@ -1246,11 +1246,11 @@
         <v>4</v>
       </c>
       <c r="G20" t="n">
-        <v>0.5169816613197327</v>
+        <v>0.9246030449867249</v>
       </c>
       <c r="H20" t="inlineStr">
         <is>
-          <t>Tópico 5: protein, approach, performance</t>
+          <t>Tópico 5: crop, soil, system</t>
         </is>
       </c>
       <c r="I20" t="inlineStr">
@@ -1284,14 +1284,14 @@
         </is>
       </c>
       <c r="F21" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="G21" t="n">
-        <v>0.4166155457496643</v>
+        <v>0.8908332586288452</v>
       </c>
       <c r="H21" t="inlineStr">
         <is>
-          <t>Tópico 1: model, nitrogen, network</t>
+          <t>Tópico 3: protein, effector, sequence</t>
         </is>
       </c>
       <c r="I21" t="inlineStr">
@@ -1325,14 +1325,14 @@
         </is>
       </c>
       <c r="F22" t="n">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="G22" t="n">
-        <v>0.7382628917694092</v>
+        <v>0.9936512112617493</v>
       </c>
       <c r="H22" t="inlineStr">
         <is>
-          <t>Tópico 6: cassava, accuracy, feature</t>
+          <t>Tópico 4: yolov, increase, map</t>
         </is>
       </c>
       <c r="I22" t="inlineStr">
@@ -1360,18 +1360,20 @@
       <c r="D23" t="n">
         <v>2025</v>
       </c>
-      <c r="E23" t="n">
-        <v>0</v>
+      <c r="E23" t="inlineStr">
+        <is>
+          <t>No especificado</t>
+        </is>
       </c>
       <c r="F23" t="n">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="G23" t="n">
-        <v>0.6001870632171631</v>
+        <v>0.5301912426948547</v>
       </c>
       <c r="H23" t="inlineStr">
         <is>
-          <t>Tópico 8: crop, soil, tomato</t>
+          <t>Tópico 6: soybean, vegetable, learningbased</t>
         </is>
       </c>
       <c r="I23" t="inlineStr">
@@ -1405,14 +1407,14 @@
         </is>
       </c>
       <c r="F24" t="n">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="G24" t="n">
-        <v>0.5007379651069641</v>
+        <v>0.5336745977401733</v>
       </c>
       <c r="H24" t="inlineStr">
         <is>
-          <t>Tópico 6: cassava, accuracy, feature</t>
+          <t>Tópico 7: model, data, study</t>
         </is>
       </c>
       <c r="I24" t="inlineStr">
@@ -1440,18 +1442,20 @@
       <c r="D25" t="n">
         <v>2025</v>
       </c>
-      <c r="E25" t="n">
-        <v>0</v>
+      <c r="E25" t="inlineStr">
+        <is>
+          <t>No especificado</t>
+        </is>
       </c>
       <c r="F25" t="n">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="G25" t="n">
-        <v>0.9926392436027527</v>
+        <v>0.5776461362838745</v>
       </c>
       <c r="H25" t="inlineStr">
         <is>
-          <t>Tópico 6: cassava, accuracy, feature</t>
+          <t>Tópico 7: model, data, study</t>
         </is>
       </c>
       <c r="I25" t="inlineStr">
@@ -1479,18 +1483,20 @@
       <c r="D26" t="n">
         <v>2025</v>
       </c>
-      <c r="E26" t="n">
+      <c r="E26" t="inlineStr">
+        <is>
+          <t>No especificado</t>
+        </is>
+      </c>
+      <c r="F26" t="n">
         <v>0</v>
       </c>
-      <c r="F26" t="n">
-        <v>5</v>
-      </c>
       <c r="G26" t="n">
-        <v>0.7574189901351929</v>
+        <v>0.4962655901908875</v>
       </c>
       <c r="H26" t="inlineStr">
         <is>
-          <t>Tópico 6: cassava, accuracy, feature</t>
+          <t>Tópico 1: cassava, blight, potato</t>
         </is>
       </c>
       <c r="I26" t="inlineStr">
@@ -1524,14 +1530,14 @@
         </is>
       </c>
       <c r="F27" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="G27" t="n">
-        <v>0.5083088874816895</v>
+        <v>0.7229164242744446</v>
       </c>
       <c r="H27" t="inlineStr">
         <is>
-          <t>Tópico 2: protein, effector, sequence</t>
+          <t>Tópico 3: protein, effector, sequence</t>
         </is>
       </c>
       <c r="I27" t="inlineStr">
@@ -1565,14 +1571,14 @@
         </is>
       </c>
       <c r="F28" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="G28" t="n">
-        <v>0.6229103207588196</v>
+        <v>0.9932265877723694</v>
       </c>
       <c r="H28" t="inlineStr">
         <is>
-          <t>Tópico 2: protein, effector, sequence</t>
+          <t>Tópico 3: protein, effector, sequence</t>
         </is>
       </c>
       <c r="I28" t="inlineStr">
@@ -1600,18 +1606,20 @@
       <c r="D29" t="n">
         <v>2025</v>
       </c>
-      <c r="E29" t="n">
-        <v>0</v>
+      <c r="E29" t="inlineStr">
+        <is>
+          <t>No especificado</t>
+        </is>
       </c>
       <c r="F29" t="n">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="G29" t="n">
-        <v>0.9878597855567932</v>
+        <v>0.7066919207572937</v>
       </c>
       <c r="H29" t="inlineStr">
         <is>
-          <t>Tópico 3: nitrogen, model, soil</t>
+          <t>Tópico 5: crop, soil, system</t>
         </is>
       </c>
       <c r="I29" t="inlineStr">
@@ -1648,11 +1656,11 @@
         <v>4</v>
       </c>
       <c r="G30" t="n">
-        <v>0.663735568523407</v>
+        <v>0.992110550403595</v>
       </c>
       <c r="H30" t="inlineStr">
         <is>
-          <t>Tópico 5: protein, approach, performance</t>
+          <t>Tópico 5: crop, soil, system</t>
         </is>
       </c>
       <c r="I30" t="inlineStr">
@@ -1680,18 +1688,20 @@
       <c r="D31" t="n">
         <v>2025</v>
       </c>
-      <c r="E31" t="n">
-        <v>0</v>
+      <c r="E31" t="inlineStr">
+        <is>
+          <t>No especificado</t>
+        </is>
       </c>
       <c r="F31" t="n">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="G31" t="n">
-        <v>0.5678712129592896</v>
+        <v>0.9949524998664856</v>
       </c>
       <c r="H31" t="inlineStr">
         <is>
-          <t>Tópico 8: crop, soil, tomato</t>
+          <t>Tópico 5: crop, soil, system</t>
         </is>
       </c>
       <c r="I31" t="inlineStr">
@@ -1719,18 +1729,20 @@
       <c r="D32" t="n">
         <v>2025</v>
       </c>
-      <c r="E32" t="n">
-        <v>0</v>
+      <c r="E32" t="inlineStr">
+        <is>
+          <t>No especificado</t>
+        </is>
       </c>
       <c r="F32" t="n">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="G32" t="n">
-        <v>0.6821849346160889</v>
+        <v>0.511612594127655</v>
       </c>
       <c r="H32" t="inlineStr">
         <is>
-          <t>Tópico 6: cassava, accuracy, feature</t>
+          <t>Tópico 7: model, data, study</t>
         </is>
       </c>
       <c r="I32" t="inlineStr">
@@ -1764,14 +1776,14 @@
         </is>
       </c>
       <c r="F33" t="n">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="G33" t="n">
-        <v>0.5000377297401428</v>
+        <v>0.7227580547332764</v>
       </c>
       <c r="H33" t="inlineStr">
         <is>
-          <t>Tópico 5: protein, approach, performance</t>
+          <t>Tópico 3: protein, effector, sequence</t>
         </is>
       </c>
       <c r="I33" t="inlineStr">
@@ -1805,14 +1817,14 @@
         </is>
       </c>
       <c r="F34" t="n">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="G34" t="n">
-        <v>0.9158463478088379</v>
+        <v>0.5282415747642517</v>
       </c>
       <c r="H34" t="inlineStr">
         <is>
-          <t>Tópico 5: protein, approach, performance</t>
+          <t>Tópico 6: soybean, vegetable, learningbased</t>
         </is>
       </c>
       <c r="I34" t="inlineStr">
@@ -1846,14 +1858,14 @@
         </is>
       </c>
       <c r="F35" t="n">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="G35" t="n">
-        <v>0.7197501063346863</v>
+        <v>0.790249764919281</v>
       </c>
       <c r="H35" t="inlineStr">
         <is>
-          <t>Tópico 4: gene, bacterial, target</t>
+          <t>Tópico 6: soybean, vegetable, learningbased</t>
         </is>
       </c>
       <c r="I35" t="inlineStr">
@@ -1887,14 +1899,14 @@
         </is>
       </c>
       <c r="F36" t="n">
-        <v>2</v>
+        <v>6</v>
       </c>
       <c r="G36" t="n">
-        <v>0.6912333369255066</v>
+        <v>0.6101933717727661</v>
       </c>
       <c r="H36" t="inlineStr">
         <is>
-          <t>Tópico 3: nitrogen, model, soil</t>
+          <t>Tópico 7: model, data, study</t>
         </is>
       </c>
       <c r="I36" t="inlineStr">
@@ -1928,14 +1940,14 @@
         </is>
       </c>
       <c r="F37" t="n">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="G37" t="n">
-        <v>0.9207252264022827</v>
+        <v>0.9941560626029968</v>
       </c>
       <c r="H37" t="inlineStr">
         <is>
-          <t>Tópico 1: model, nitrogen, network</t>
+          <t>Tópico 5: crop, soil, system</t>
         </is>
       </c>
       <c r="I37" t="inlineStr">
@@ -1969,14 +1981,14 @@
         </is>
       </c>
       <c r="F38" t="n">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="G38" t="n">
-        <v>0.5134923458099365</v>
+        <v>0.9200223088264465</v>
       </c>
       <c r="H38" t="inlineStr">
         <is>
-          <t>Tópico 3: nitrogen, model, soil</t>
+          <t>Tópico 5: crop, soil, system</t>
         </is>
       </c>
       <c r="I38" t="inlineStr">
@@ -2010,14 +2022,14 @@
         </is>
       </c>
       <c r="F39" t="n">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="G39" t="n">
-        <v>0.7979367971420288</v>
+        <v>0.4643924236297607</v>
       </c>
       <c r="H39" t="inlineStr">
         <is>
-          <t>Tópico 6: cassava, accuracy, feature</t>
+          <t>Tópico 7: model, data, study</t>
         </is>
       </c>
       <c r="I39" t="inlineStr">
@@ -2051,14 +2063,14 @@
         </is>
       </c>
       <c r="F40" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="G40" t="n">
-        <v>0.3744944036006927</v>
+        <v>0.8757714629173279</v>
       </c>
       <c r="H40" t="inlineStr">
         <is>
-          <t>Tópico 2: protein, effector, sequence</t>
+          <t>Tópico 4: yolov, increase, map</t>
         </is>
       </c>
       <c r="I40" t="inlineStr">
@@ -2095,11 +2107,11 @@
         <v>2</v>
       </c>
       <c r="G41" t="n">
-        <v>0.6908019781112671</v>
+        <v>0.9375365972518921</v>
       </c>
       <c r="H41" t="inlineStr">
         <is>
-          <t>Tópico 3: nitrogen, model, soil</t>
+          <t>Tópico 3: protein, effector, sequence</t>
         </is>
       </c>
       <c r="I41" t="inlineStr">
@@ -2133,14 +2145,14 @@
         </is>
       </c>
       <c r="F42" t="n">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="G42" t="n">
-        <v>0.3812733292579651</v>
+        <v>0.5971952080726624</v>
       </c>
       <c r="H42" t="inlineStr">
         <is>
-          <t>Tópico 8: crop, soil, tomato</t>
+          <t>Tópico 5: crop, soil, system</t>
         </is>
       </c>
       <c r="I42" t="inlineStr">
@@ -2174,14 +2186,14 @@
         </is>
       </c>
       <c r="F43" t="n">
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="G43" t="n">
-        <v>0.7350122928619385</v>
+        <v>0.5263422727584839</v>
       </c>
       <c r="H43" t="inlineStr">
         <is>
-          <t>Tópico 6: cassava, accuracy, feature</t>
+          <t>Tópico 1: cassava, blight, potato</t>
         </is>
       </c>
       <c r="I43" t="inlineStr">
@@ -2215,14 +2227,14 @@
         </is>
       </c>
       <c r="F44" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="G44" t="n">
-        <v>0.6559547781944275</v>
+        <v>0.6387072205543518</v>
       </c>
       <c r="H44" t="inlineStr">
         <is>
-          <t>Tópico 6: cassava, accuracy, feature</t>
+          <t>Tópico 5: crop, soil, system</t>
         </is>
       </c>
       <c r="I44" t="inlineStr">
@@ -2256,14 +2268,14 @@
         </is>
       </c>
       <c r="F45" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="G45" t="n">
-        <v>0.8826786279678345</v>
+        <v>0.991178035736084</v>
       </c>
       <c r="H45" t="inlineStr">
         <is>
-          <t>Tópico 2: protein, effector, sequence</t>
+          <t>Tópico 3: protein, effector, sequence</t>
         </is>
       </c>
       <c r="I45" t="inlineStr">
@@ -2297,14 +2309,14 @@
         </is>
       </c>
       <c r="F46" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="G46" t="n">
-        <v>0.4422743618488312</v>
+        <v>0.3967302441596985</v>
       </c>
       <c r="H46" t="inlineStr">
         <is>
-          <t>Tópico 6: cassava, accuracy, feature</t>
+          <t>Tópico 5: crop, soil, system</t>
         </is>
       </c>
       <c r="I46" t="inlineStr">
@@ -2338,14 +2350,14 @@
         </is>
       </c>
       <c r="F47" t="n">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="G47" t="n">
-        <v>0.9924623966217041</v>
+        <v>0.9928716421127319</v>
       </c>
       <c r="H47" t="inlineStr">
         <is>
-          <t>Tópico 8: crop, soil, tomato</t>
+          <t>Tópico 5: crop, soil, system</t>
         </is>
       </c>
       <c r="I47" t="inlineStr">
@@ -2379,14 +2391,14 @@
         </is>
       </c>
       <c r="F48" t="n">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="G48" t="n">
-        <v>0.474578320980072</v>
+        <v>0.6912403106689453</v>
       </c>
       <c r="H48" t="inlineStr">
         <is>
-          <t>Tópico 3: nitrogen, model, soil</t>
+          <t>Tópico 6: soybean, vegetable, learningbased</t>
         </is>
       </c>
       <c r="I48" t="inlineStr">
@@ -2420,14 +2432,14 @@
         </is>
       </c>
       <c r="F49" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="G49" t="n">
-        <v>0.992637038230896</v>
+        <v>0.9924727082252502</v>
       </c>
       <c r="H49" t="inlineStr">
         <is>
-          <t>Tópico 4: gene, bacterial, target</t>
+          <t>Tópico 3: protein, effector, sequence</t>
         </is>
       </c>
       <c r="I49" t="inlineStr">
@@ -2461,14 +2473,14 @@
         </is>
       </c>
       <c r="F50" t="n">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="G50" t="n">
-        <v>0.5819512605667114</v>
+        <v>0.8176574110984802</v>
       </c>
       <c r="H50" t="inlineStr">
         <is>
-          <t>Tópico 8: crop, soil, tomato</t>
+          <t>Tópico 5: crop, soil, system</t>
         </is>
       </c>
       <c r="I50" t="inlineStr">
@@ -2502,14 +2514,14 @@
         </is>
       </c>
       <c r="F51" t="n">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="G51" t="n">
-        <v>0.8627616763114929</v>
+        <v>0.9920365214347839</v>
       </c>
       <c r="H51" t="inlineStr">
         <is>
-          <t>Tópico 6: cassava, accuracy, feature</t>
+          <t>Tópico 2: tomato, fruit, grape</t>
         </is>
       </c>
       <c r="I51" t="inlineStr">
@@ -2543,14 +2555,14 @@
         </is>
       </c>
       <c r="F52" t="n">
-        <v>2</v>
+        <v>6</v>
       </c>
       <c r="G52" t="n">
-        <v>0.47402423620224</v>
+        <v>0.4786550104618073</v>
       </c>
       <c r="H52" t="inlineStr">
         <is>
-          <t>Tópico 3: nitrogen, model, soil</t>
+          <t>Tópico 7: model, data, study</t>
         </is>
       </c>
       <c r="I52" t="inlineStr">
@@ -2584,14 +2596,14 @@
         </is>
       </c>
       <c r="F53" t="n">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="G53" t="n">
-        <v>0.992438793182373</v>
+        <v>0.3863027095794678</v>
       </c>
       <c r="H53" t="inlineStr">
         <is>
-          <t>Tópico 6: cassava, accuracy, feature</t>
+          <t>Tópico 4: yolov, increase, map</t>
         </is>
       </c>
       <c r="I53" t="inlineStr">
@@ -2625,14 +2637,14 @@
         </is>
       </c>
       <c r="F54" t="n">
-        <v>6</v>
+        <v>0</v>
       </c>
       <c r="G54" t="n">
-        <v>0.8148534893989563</v>
+        <v>0.6947838068008423</v>
       </c>
       <c r="H54" t="inlineStr">
         <is>
-          <t>Tópico 7: potato, blight, hyperspectral</t>
+          <t>Tópico 1: cassava, blight, potato</t>
         </is>
       </c>
       <c r="I54" t="inlineStr">
@@ -2660,18 +2672,20 @@
       <c r="D55" t="n">
         <v>2024</v>
       </c>
-      <c r="E55" t="n">
-        <v>0</v>
+      <c r="E55" t="inlineStr">
+        <is>
+          <t>No especificado</t>
+        </is>
       </c>
       <c r="F55" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="G55" t="n">
-        <v>0.9908462762832642</v>
+        <v>0.6322852373123169</v>
       </c>
       <c r="H55" t="inlineStr">
         <is>
-          <t>Tópico 1: model, nitrogen, network</t>
+          <t>Tópico 3: protein, effector, sequence</t>
         </is>
       </c>
       <c r="I55" t="inlineStr">
@@ -2699,18 +2713,20 @@
       <c r="D56" t="n">
         <v>2024</v>
       </c>
-      <c r="E56" t="n">
-        <v>0</v>
+      <c r="E56" t="inlineStr">
+        <is>
+          <t>No especificado</t>
+        </is>
       </c>
       <c r="F56" t="n">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="G56" t="n">
-        <v>0.8897254467010498</v>
+        <v>0.7513718008995056</v>
       </c>
       <c r="H56" t="inlineStr">
         <is>
-          <t>Tópico 8: crop, soil, tomato</t>
+          <t>Tópico 5: crop, soil, system</t>
         </is>
       </c>
       <c r="I56" t="inlineStr">
@@ -2738,18 +2754,20 @@
       <c r="D57" t="n">
         <v>2024</v>
       </c>
-      <c r="E57" t="n">
-        <v>0</v>
+      <c r="E57" t="inlineStr">
+        <is>
+          <t>No especificado</t>
+        </is>
       </c>
       <c r="F57" t="n">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="G57" t="n">
-        <v>0.5845791697502136</v>
+        <v>0.6681990623474121</v>
       </c>
       <c r="H57" t="inlineStr">
         <is>
-          <t>Tópico 1: model, nitrogen, network</t>
+          <t>Tópico 5: crop, soil, system</t>
         </is>
       </c>
       <c r="I57" t="inlineStr">
@@ -2777,18 +2795,20 @@
       <c r="D58" t="n">
         <v>2024</v>
       </c>
-      <c r="E58" t="n">
-        <v>0</v>
+      <c r="E58" t="inlineStr">
+        <is>
+          <t>No especificado</t>
+        </is>
       </c>
       <c r="F58" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="G58" t="n">
-        <v>0.6622006297111511</v>
+        <v>0.9892328977584839</v>
       </c>
       <c r="H58" t="inlineStr">
         <is>
-          <t>Tópico 8: crop, soil, tomato</t>
+          <t>Tópico 7: model, data, study</t>
         </is>
       </c>
       <c r="I58" t="inlineStr">
@@ -2822,14 +2842,14 @@
         </is>
       </c>
       <c r="F59" t="n">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="G59" t="n">
-        <v>0.627256453037262</v>
+        <v>0.9935283064842224</v>
       </c>
       <c r="H59" t="inlineStr">
         <is>
-          <t>Tópico 5: protein, approach, performance</t>
+          <t>Tópico 6: soybean, vegetable, learningbased</t>
         </is>
       </c>
       <c r="I59" t="inlineStr">
@@ -2863,14 +2883,14 @@
         </is>
       </c>
       <c r="F60" t="n">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="G60" t="n">
-        <v>0.9358692169189453</v>
+        <v>0.9966049194335938</v>
       </c>
       <c r="H60" t="inlineStr">
         <is>
-          <t>Tópico 1: model, nitrogen, network</t>
+          <t>Tópico 5: crop, soil, system</t>
         </is>
       </c>
       <c r="I60" t="inlineStr">
@@ -2904,14 +2924,14 @@
         </is>
       </c>
       <c r="F61" t="n">
-        <v>7</v>
+        <v>1</v>
       </c>
       <c r="G61" t="n">
-        <v>0.4817582368850708</v>
+        <v>0.5148641467094421</v>
       </c>
       <c r="H61" t="inlineStr">
         <is>
-          <t>Tópico 8: crop, soil, tomato</t>
+          <t>Tópico 2: tomato, fruit, grape</t>
         </is>
       </c>
       <c r="I61" t="inlineStr">
@@ -2939,18 +2959,20 @@
       <c r="D62" t="n">
         <v>2024</v>
       </c>
-      <c r="E62" t="n">
-        <v>0</v>
+      <c r="E62" t="inlineStr">
+        <is>
+          <t>No especificado</t>
+        </is>
       </c>
       <c r="F62" t="n">
-        <v>7</v>
+        <v>1</v>
       </c>
       <c r="G62" t="n">
-        <v>0.994579553604126</v>
+        <v>0.993289589881897</v>
       </c>
       <c r="H62" t="inlineStr">
         <is>
-          <t>Tópico 8: crop, soil, tomato</t>
+          <t>Tópico 2: tomato, fruit, grape</t>
         </is>
       </c>
       <c r="I62" t="inlineStr">
@@ -2984,14 +3006,14 @@
         </is>
       </c>
       <c r="F63" t="n">
-        <v>2</v>
+        <v>6</v>
       </c>
       <c r="G63" t="n">
-        <v>0.4111634790897369</v>
+        <v>0.6559443473815918</v>
       </c>
       <c r="H63" t="inlineStr">
         <is>
-          <t>Tópico 3: nitrogen, model, soil</t>
+          <t>Tópico 7: model, data, study</t>
         </is>
       </c>
       <c r="I63" t="inlineStr">
@@ -3019,18 +3041,20 @@
       <c r="D64" t="n">
         <v>2024</v>
       </c>
-      <c r="E64" t="n">
-        <v>0</v>
+      <c r="E64" t="inlineStr">
+        <is>
+          <t>No especificado</t>
+        </is>
       </c>
       <c r="F64" t="n">
         <v>5</v>
       </c>
       <c r="G64" t="n">
-        <v>0.9948951601982117</v>
+        <v>0.4008100926876068</v>
       </c>
       <c r="H64" t="inlineStr">
         <is>
-          <t>Tópico 6: cassava, accuracy, feature</t>
+          <t>Tópico 6: soybean, vegetable, learningbased</t>
         </is>
       </c>
       <c r="I64" t="inlineStr">
@@ -3064,14 +3088,14 @@
         </is>
       </c>
       <c r="F65" t="n">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="G65" t="n">
-        <v>0.9954486489295959</v>
+        <v>0.9957056045532227</v>
       </c>
       <c r="H65" t="inlineStr">
         <is>
-          <t>Tópico 8: crop, soil, tomato</t>
+          <t>Tópico 5: crop, soil, system</t>
         </is>
       </c>
       <c r="I65" t="inlineStr">
@@ -3105,14 +3129,14 @@
         </is>
       </c>
       <c r="F66" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="G66" t="n">
-        <v>0.6897719502449036</v>
+        <v>0.5935820937156677</v>
       </c>
       <c r="H66" t="inlineStr">
         <is>
-          <t>Tópico 2: protein, effector, sequence</t>
+          <t>Tópico 3: protein, effector, sequence</t>
         </is>
       </c>
       <c r="I66" t="inlineStr">
@@ -3146,14 +3170,14 @@
         </is>
       </c>
       <c r="F67" t="n">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="G67" t="n">
-        <v>0.3863769471645355</v>
+        <v>0.6031487584114075</v>
       </c>
       <c r="H67" t="inlineStr">
         <is>
-          <t>Tópico 6: cassava, accuracy, feature</t>
+          <t>Tópico 3: protein, effector, sequence</t>
         </is>
       </c>
       <c r="I67" t="inlineStr">
@@ -3190,11 +3214,11 @@
         <v>6</v>
       </c>
       <c r="G68" t="n">
-        <v>0.9930324554443359</v>
+        <v>0.6631643176078796</v>
       </c>
       <c r="H68" t="inlineStr">
         <is>
-          <t>Tópico 7: potato, blight, hyperspectral</t>
+          <t>Tópico 7: model, data, study</t>
         </is>
       </c>
       <c r="I68" t="inlineStr">
@@ -3228,14 +3252,14 @@
         </is>
       </c>
       <c r="F69" t="n">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="G69" t="n">
-        <v>0.8844049572944641</v>
+        <v>0.2826882600784302</v>
       </c>
       <c r="H69" t="inlineStr">
         <is>
-          <t>Tópico 6: cassava, accuracy, feature</t>
+          <t>Tópico 2: tomato, fruit, grape</t>
         </is>
       </c>
       <c r="I69" t="inlineStr">
@@ -3263,18 +3287,20 @@
       <c r="D70" t="n">
         <v>2024</v>
       </c>
-      <c r="E70" t="n">
-        <v>0</v>
+      <c r="E70" t="inlineStr">
+        <is>
+          <t>No especificado</t>
+        </is>
       </c>
       <c r="F70" t="n">
         <v>4</v>
       </c>
       <c r="G70" t="n">
-        <v>0.4783314764499664</v>
+        <v>0.3637583255767822</v>
       </c>
       <c r="H70" t="inlineStr">
         <is>
-          <t>Tópico 5: protein, approach, performance</t>
+          <t>Tópico 5: crop, soil, system</t>
         </is>
       </c>
       <c r="I70" t="inlineStr">
@@ -3308,14 +3334,14 @@
         </is>
       </c>
       <c r="F71" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="G71" t="n">
-        <v>0.9912151694297791</v>
+        <v>0.8396974802017212</v>
       </c>
       <c r="H71" t="inlineStr">
         <is>
-          <t>Tópico 4: gene, bacterial, target</t>
+          <t>Tópico 3: protein, effector, sequence</t>
         </is>
       </c>
       <c r="I71" t="inlineStr">
@@ -3349,14 +3375,14 @@
         </is>
       </c>
       <c r="F72" t="n">
-        <v>2</v>
+        <v>6</v>
       </c>
       <c r="G72" t="n">
-        <v>0.9947726726531982</v>
+        <v>0.6541068553924561</v>
       </c>
       <c r="H72" t="inlineStr">
         <is>
-          <t>Tópico 3: nitrogen, model, soil</t>
+          <t>Tópico 7: model, data, study</t>
         </is>
       </c>
       <c r="I72" t="inlineStr">
@@ -3390,14 +3416,14 @@
         </is>
       </c>
       <c r="F73" t="n">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="G73" t="n">
-        <v>0.9934744238853455</v>
+        <v>0.9010332226753235</v>
       </c>
       <c r="H73" t="inlineStr">
         <is>
-          <t>Tópico 3: nitrogen, model, soil</t>
+          <t>Tópico 5: crop, soil, system</t>
         </is>
       </c>
       <c r="I73" t="inlineStr">
@@ -3431,14 +3457,14 @@
         </is>
       </c>
       <c r="F74" t="n">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="G74" t="n">
-        <v>0.9903035759925842</v>
+        <v>0.9882709383964539</v>
       </c>
       <c r="H74" t="inlineStr">
         <is>
-          <t>Tópico 6: cassava, accuracy, feature</t>
+          <t>Tópico 7: model, data, study</t>
         </is>
       </c>
       <c r="I74" t="inlineStr">
@@ -3472,14 +3498,14 @@
         </is>
       </c>
       <c r="F75" t="n">
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="G75" t="n">
-        <v>0.993352472782135</v>
+        <v>0.3946555554866791</v>
       </c>
       <c r="H75" t="inlineStr">
         <is>
-          <t>Tópico 6: cassava, accuracy, feature</t>
+          <t>Tópico 1: cassava, blight, potato</t>
         </is>
       </c>
       <c r="I75" t="inlineStr">
@@ -3513,14 +3539,14 @@
         </is>
       </c>
       <c r="F76" t="n">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="G76" t="n">
-        <v>0.7874866724014282</v>
+        <v>0.925505518913269</v>
       </c>
       <c r="H76" t="inlineStr">
         <is>
-          <t>Tópico 3: nitrogen, model, soil</t>
+          <t>Tópico 5: crop, soil, system</t>
         </is>
       </c>
       <c r="I76" t="inlineStr">
@@ -3554,14 +3580,14 @@
         </is>
       </c>
       <c r="F77" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="G77" t="n">
-        <v>0.5155216455459595</v>
+        <v>0.7359481453895569</v>
       </c>
       <c r="H77" t="inlineStr">
         <is>
-          <t>Tópico 1: model, nitrogen, network</t>
+          <t>Tópico 3: protein, effector, sequence</t>
         </is>
       </c>
       <c r="I77" t="inlineStr">
@@ -3595,14 +3621,14 @@
         </is>
       </c>
       <c r="F78" t="n">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="G78" t="n">
-        <v>0.6214307546615601</v>
+        <v>0.9295258522033691</v>
       </c>
       <c r="H78" t="inlineStr">
         <is>
-          <t>Tópico 5: protein, approach, performance</t>
+          <t>Tópico 2: tomato, fruit, grape</t>
         </is>
       </c>
       <c r="I78" t="inlineStr">
@@ -3636,14 +3662,14 @@
         </is>
       </c>
       <c r="F79" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="G79" t="n">
-        <v>0.7585625052452087</v>
+        <v>0.6701561808586121</v>
       </c>
       <c r="H79" t="inlineStr">
         <is>
-          <t>Tópico 2: protein, effector, sequence</t>
+          <t>Tópico 3: protein, effector, sequence</t>
         </is>
       </c>
       <c r="I79" t="inlineStr">
@@ -3680,11 +3706,11 @@
         <v>0</v>
       </c>
       <c r="G80" t="n">
-        <v>0.6102871298789978</v>
+        <v>0.649029552936554</v>
       </c>
       <c r="H80" t="inlineStr">
         <is>
-          <t>Tópico 1: model, nitrogen, network</t>
+          <t>Tópico 1: cassava, blight, potato</t>
         </is>
       </c>
       <c r="I80" t="inlineStr">
@@ -3718,14 +3744,14 @@
         </is>
       </c>
       <c r="F81" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G81" t="n">
-        <v>0.445617139339447</v>
+        <v>0.4267955720424652</v>
       </c>
       <c r="H81" t="inlineStr">
         <is>
-          <t>Tópico 2: protein, effector, sequence</t>
+          <t>Tópico 1: cassava, blight, potato</t>
         </is>
       </c>
       <c r="I81" t="inlineStr">
@@ -3759,14 +3785,14 @@
         </is>
       </c>
       <c r="F82" t="n">
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="G82" t="n">
-        <v>0.4063605964183807</v>
+        <v>0.79137122631073</v>
       </c>
       <c r="H82" t="inlineStr">
         <is>
-          <t>Tópico 6: cassava, accuracy, feature</t>
+          <t>Tópico 1: cassava, blight, potato</t>
         </is>
       </c>
       <c r="I82" t="inlineStr">
@@ -3800,14 +3826,14 @@
         </is>
       </c>
       <c r="F83" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="G83" t="n">
-        <v>0.5983458161354065</v>
+        <v>0.4137524962425232</v>
       </c>
       <c r="H83" t="inlineStr">
         <is>
-          <t>Tópico 6: cassava, accuracy, feature</t>
+          <t>Tópico 5: crop, soil, system</t>
         </is>
       </c>
       <c r="I83" t="inlineStr">
@@ -3835,18 +3861,20 @@
       <c r="D84" t="n">
         <v>2023</v>
       </c>
-      <c r="E84" t="n">
-        <v>0</v>
+      <c r="E84" t="inlineStr">
+        <is>
+          <t>No especificado</t>
+        </is>
       </c>
       <c r="F84" t="n">
-        <v>7</v>
+        <v>1</v>
       </c>
       <c r="G84" t="n">
-        <v>0.9928593039512634</v>
+        <v>0.8859900236129761</v>
       </c>
       <c r="H84" t="inlineStr">
         <is>
-          <t>Tópico 8: crop, soil, tomato</t>
+          <t>Tópico 2: tomato, fruit, grape</t>
         </is>
       </c>
       <c r="I84" t="inlineStr">
@@ -3874,18 +3902,20 @@
       <c r="D85" t="n">
         <v>2023</v>
       </c>
-      <c r="E85" t="n">
-        <v>0</v>
+      <c r="E85" t="inlineStr">
+        <is>
+          <t>No especificado</t>
+        </is>
       </c>
       <c r="F85" t="n">
         <v>4</v>
       </c>
       <c r="G85" t="n">
-        <v>0.6040872931480408</v>
+        <v>0.6794548034667969</v>
       </c>
       <c r="H85" t="inlineStr">
         <is>
-          <t>Tópico 5: protein, approach, performance</t>
+          <t>Tópico 5: crop, soil, system</t>
         </is>
       </c>
       <c r="I85" t="inlineStr">
@@ -3913,18 +3943,20 @@
       <c r="D86" t="n">
         <v>2023</v>
       </c>
-      <c r="E86" t="n">
-        <v>0</v>
+      <c r="E86" t="inlineStr">
+        <is>
+          <t>No especificado</t>
+        </is>
       </c>
       <c r="F86" t="n">
         <v>5</v>
       </c>
       <c r="G86" t="n">
-        <v>0.8656045198440552</v>
+        <v>0.3512542843818665</v>
       </c>
       <c r="H86" t="inlineStr">
         <is>
-          <t>Tópico 6: cassava, accuracy, feature</t>
+          <t>Tópico 6: soybean, vegetable, learningbased</t>
         </is>
       </c>
       <c r="I86" t="inlineStr">
@@ -3952,18 +3984,20 @@
       <c r="D87" t="n">
         <v>2023</v>
       </c>
-      <c r="E87" t="n">
-        <v>0</v>
+      <c r="E87" t="inlineStr">
+        <is>
+          <t>No especificado</t>
+        </is>
       </c>
       <c r="F87" t="n">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="G87" t="n">
-        <v>0.9918966293334961</v>
+        <v>0.4628013074398041</v>
       </c>
       <c r="H87" t="inlineStr">
         <is>
-          <t>Tópico 8: crop, soil, tomato</t>
+          <t>Tópico 5: crop, soil, system</t>
         </is>
       </c>
       <c r="I87" t="inlineStr">
@@ -3997,14 +4031,14 @@
         </is>
       </c>
       <c r="F88" t="n">
-        <v>2</v>
+        <v>6</v>
       </c>
       <c r="G88" t="n">
-        <v>0.5486451983451843</v>
+        <v>0.5343393087387085</v>
       </c>
       <c r="H88" t="inlineStr">
         <is>
-          <t>Tópico 3: nitrogen, model, soil</t>
+          <t>Tópico 7: model, data, study</t>
         </is>
       </c>
       <c r="I88" t="inlineStr">
@@ -4038,14 +4072,14 @@
         </is>
       </c>
       <c r="F89" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G89" t="n">
-        <v>0.4073373675346375</v>
+        <v>0.5130228400230408</v>
       </c>
       <c r="H89" t="inlineStr">
         <is>
-          <t>Tópico 2: protein, effector, sequence</t>
+          <t>Tópico 1: cassava, blight, potato</t>
         </is>
       </c>
       <c r="I89" t="inlineStr">
@@ -4079,14 +4113,14 @@
         </is>
       </c>
       <c r="F90" t="n">
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="G90" t="n">
-        <v>0.4306102395057678</v>
+        <v>0.5654139518737793</v>
       </c>
       <c r="H90" t="inlineStr">
         <is>
-          <t>Tópico 6: cassava, accuracy, feature</t>
+          <t>Tópico 1: cassava, blight, potato</t>
         </is>
       </c>
       <c r="I90" t="inlineStr">
@@ -4114,18 +4148,20 @@
       <c r="D91" t="n">
         <v>2023</v>
       </c>
-      <c r="E91" t="n">
-        <v>0</v>
+      <c r="E91" t="inlineStr">
+        <is>
+          <t>No especificado</t>
+        </is>
       </c>
       <c r="F91" t="n">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="G91" t="n">
-        <v>0.9918977022171021</v>
+        <v>0.5699195861816406</v>
       </c>
       <c r="H91" t="inlineStr">
         <is>
-          <t>Tópico 8: crop, soil, tomato</t>
+          <t>Tópico 5: crop, soil, system</t>
         </is>
       </c>
       <c r="I91" t="inlineStr">
@@ -4153,18 +4189,20 @@
       <c r="D92" t="n">
         <v>2023</v>
       </c>
-      <c r="E92" t="n">
-        <v>0</v>
+      <c r="E92" t="inlineStr">
+        <is>
+          <t>No especificado</t>
+        </is>
       </c>
       <c r="F92" t="n">
-        <v>7</v>
+        <v>1</v>
       </c>
       <c r="G92" t="n">
-        <v>0.4602072238922119</v>
+        <v>0.7834851741790771</v>
       </c>
       <c r="H92" t="inlineStr">
         <is>
-          <t>Tópico 8: crop, soil, tomato</t>
+          <t>Tópico 2: tomato, fruit, grape</t>
         </is>
       </c>
       <c r="I92" t="inlineStr">
@@ -4198,14 +4236,14 @@
         </is>
       </c>
       <c r="F93" t="n">
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="G93" t="n">
-        <v>0.8075741529464722</v>
+        <v>0.7319851517677307</v>
       </c>
       <c r="H93" t="inlineStr">
         <is>
-          <t>Tópico 6: cassava, accuracy, feature</t>
+          <t>Tópico 1: cassava, blight, potato</t>
         </is>
       </c>
       <c r="I93" t="inlineStr">
@@ -4239,14 +4277,14 @@
         </is>
       </c>
       <c r="F94" t="n">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="G94" t="n">
-        <v>0.4516164362430573</v>
+        <v>0.4867905378341675</v>
       </c>
       <c r="H94" t="inlineStr">
         <is>
-          <t>Tópico 6: cassava, accuracy, feature</t>
+          <t>Tópico 7: model, data, study</t>
         </is>
       </c>
       <c r="I94" t="inlineStr">
@@ -4280,14 +4318,14 @@
         </is>
       </c>
       <c r="F95" t="n">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="G95" t="n">
-        <v>0.3892252743244171</v>
+        <v>0.8926389217376709</v>
       </c>
       <c r="H95" t="inlineStr">
         <is>
-          <t>Tópico 3: nitrogen, model, soil</t>
+          <t>Tópico 5: crop, soil, system</t>
         </is>
       </c>
       <c r="I95" t="inlineStr">
@@ -4315,18 +4353,20 @@
       <c r="D96" t="n">
         <v>2023</v>
       </c>
-      <c r="E96" t="n">
-        <v>0</v>
+      <c r="E96" t="inlineStr">
+        <is>
+          <t>No especificado</t>
+        </is>
       </c>
       <c r="F96" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="G96" t="n">
-        <v>0.780045747756958</v>
+        <v>0.4911169111728668</v>
       </c>
       <c r="H96" t="inlineStr">
         <is>
-          <t>Tópico 6: cassava, accuracy, feature</t>
+          <t>Tópico 5: crop, soil, system</t>
         </is>
       </c>
       <c r="I96" t="inlineStr">
@@ -4360,14 +4400,14 @@
         </is>
       </c>
       <c r="F97" t="n">
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="G97" t="n">
-        <v>0.8185713291168213</v>
+        <v>0.328843891620636</v>
       </c>
       <c r="H97" t="inlineStr">
         <is>
-          <t>Tópico 6: cassava, accuracy, feature</t>
+          <t>Tópico 1: cassava, blight, potato</t>
         </is>
       </c>
       <c r="I97" t="inlineStr">
@@ -4401,14 +4441,14 @@
         </is>
       </c>
       <c r="F98" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="G98" t="n">
-        <v>0.8741922378540039</v>
+        <v>0.8389540314674377</v>
       </c>
       <c r="H98" t="inlineStr">
         <is>
-          <t>Tópico 2: protein, effector, sequence</t>
+          <t>Tópico 3: protein, effector, sequence</t>
         </is>
       </c>
       <c r="I98" t="inlineStr">
@@ -4442,14 +4482,14 @@
         </is>
       </c>
       <c r="F99" t="n">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="G99" t="n">
-        <v>0.6190128326416016</v>
+        <v>0.796586275100708</v>
       </c>
       <c r="H99" t="inlineStr">
         <is>
-          <t>Tópico 8: crop, soil, tomato</t>
+          <t>Tópico 5: crop, soil, system</t>
         </is>
       </c>
       <c r="I99" t="inlineStr">
@@ -4477,18 +4517,20 @@
       <c r="D100" t="n">
         <v>2023</v>
       </c>
-      <c r="E100" t="n">
-        <v>0</v>
+      <c r="E100" t="inlineStr">
+        <is>
+          <t>No especificado</t>
+        </is>
       </c>
       <c r="F100" t="n">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="G100" t="n">
-        <v>0.5122842192649841</v>
+        <v>0.7037473320960999</v>
       </c>
       <c r="H100" t="inlineStr">
         <is>
-          <t>Tópico 6: cassava, accuracy, feature</t>
+          <t>Tópico 7: model, data, study</t>
         </is>
       </c>
       <c r="I100" t="inlineStr">
@@ -4522,14 +4564,14 @@
         </is>
       </c>
       <c r="F101" t="n">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="G101" t="n">
-        <v>0.5922775864601135</v>
+        <v>0.9951870441436768</v>
       </c>
       <c r="H101" t="inlineStr">
         <is>
-          <t>Tópico 8: crop, soil, tomato</t>
+          <t>Tópico 5: crop, soil, system</t>
         </is>
       </c>
       <c r="I101" t="inlineStr">
@@ -4563,14 +4605,14 @@
         </is>
       </c>
       <c r="F102" t="n">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="G102" t="n">
-        <v>0.6265881061553955</v>
+        <v>0.4780805110931396</v>
       </c>
       <c r="H102" t="inlineStr">
         <is>
-          <t>Tópico 8: crop, soil, tomato</t>
+          <t>Tópico 5: crop, soil, system</t>
         </is>
       </c>
       <c r="I102" t="inlineStr">
@@ -4604,14 +4646,14 @@
         </is>
       </c>
       <c r="F103" t="n">
-        <v>2</v>
+        <v>6</v>
       </c>
       <c r="G103" t="n">
-        <v>0.4735226035118103</v>
+        <v>0.5302886962890625</v>
       </c>
       <c r="H103" t="inlineStr">
         <is>
-          <t>Tópico 3: nitrogen, model, soil</t>
+          <t>Tópico 7: model, data, study</t>
         </is>
       </c>
       <c r="I103" t="inlineStr">
@@ -4645,14 +4687,14 @@
         </is>
       </c>
       <c r="F104" t="n">
-        <v>7</v>
+        <v>1</v>
       </c>
       <c r="G104" t="n">
-        <v>0.6656808257102966</v>
+        <v>0.5277950167655945</v>
       </c>
       <c r="H104" t="inlineStr">
         <is>
-          <t>Tópico 8: crop, soil, tomato</t>
+          <t>Tópico 2: tomato, fruit, grape</t>
         </is>
       </c>
       <c r="I104" t="inlineStr">
@@ -4686,14 +4728,14 @@
         </is>
       </c>
       <c r="F105" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="G105" t="n">
-        <v>0.49161696434021</v>
+        <v>0.5543388724327087</v>
       </c>
       <c r="H105" t="inlineStr">
         <is>
-          <t>Tópico 8: crop, soil, tomato</t>
+          <t>Tópico 7: model, data, study</t>
         </is>
       </c>
       <c r="I105" t="inlineStr">
@@ -4727,14 +4769,14 @@
         </is>
       </c>
       <c r="F106" t="n">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="G106" t="n">
-        <v>0.7634450197219849</v>
+        <v>0.4738219678401947</v>
       </c>
       <c r="H106" t="inlineStr">
         <is>
-          <t>Tópico 8: crop, soil, tomato</t>
+          <t>Tópico 5: crop, soil, system</t>
         </is>
       </c>
       <c r="I106" t="inlineStr">
@@ -4768,14 +4810,14 @@
         </is>
       </c>
       <c r="F107" t="n">
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="G107" t="n">
-        <v>0.6235883235931396</v>
+        <v>0.4689224064350128</v>
       </c>
       <c r="H107" t="inlineStr">
         <is>
-          <t>Tópico 1: model, nitrogen, network</t>
+          <t>Tópico 7: model, data, study</t>
         </is>
       </c>
       <c r="I107" t="inlineStr">
@@ -4803,18 +4845,20 @@
       <c r="D108" t="n">
         <v>2022</v>
       </c>
-      <c r="E108" t="n">
-        <v>0</v>
+      <c r="E108" t="inlineStr">
+        <is>
+          <t>No especificado</t>
+        </is>
       </c>
       <c r="F108" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="G108" t="n">
-        <v>0.5936331152915955</v>
+        <v>0.457623302936554</v>
       </c>
       <c r="H108" t="inlineStr">
         <is>
-          <t>Tópico 6: cassava, accuracy, feature</t>
+          <t>Tópico 5: crop, soil, system</t>
         </is>
       </c>
       <c r="I108" t="inlineStr">
@@ -4848,14 +4892,14 @@
         </is>
       </c>
       <c r="F109" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="G109" t="n">
-        <v>0.4679929614067078</v>
+        <v>0.9478254318237305</v>
       </c>
       <c r="H109" t="inlineStr">
         <is>
-          <t>Tópico 2: protein, effector, sequence</t>
+          <t>Tópico 3: protein, effector, sequence</t>
         </is>
       </c>
       <c r="I109" t="inlineStr">
@@ -4889,14 +4933,14 @@
         </is>
       </c>
       <c r="F110" t="n">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="G110" t="n">
-        <v>0.5025733709335327</v>
+        <v>0.7388099431991577</v>
       </c>
       <c r="H110" t="inlineStr">
         <is>
-          <t>Tópico 5: protein, approach, performance</t>
+          <t>Tópico 2: tomato, fruit, grape</t>
         </is>
       </c>
       <c r="I110" t="inlineStr">
@@ -4930,14 +4974,14 @@
         </is>
       </c>
       <c r="F111" t="n">
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="G111" t="n">
-        <v>0.781898021697998</v>
+        <v>0.3819758296012878</v>
       </c>
       <c r="H111" t="inlineStr">
         <is>
-          <t>Tópico 6: cassava, accuracy, feature</t>
+          <t>Tópico 1: cassava, blight, potato</t>
         </is>
       </c>
       <c r="I111" t="inlineStr">
@@ -4974,11 +5018,11 @@
         <v>5</v>
       </c>
       <c r="G112" t="n">
-        <v>0.3614128232002258</v>
+        <v>0.4609563052654266</v>
       </c>
       <c r="H112" t="inlineStr">
         <is>
-          <t>Tópico 6: cassava, accuracy, feature</t>
+          <t>Tópico 6: soybean, vegetable, learningbased</t>
         </is>
       </c>
       <c r="I112" t="inlineStr">
@@ -5012,14 +5056,14 @@
         </is>
       </c>
       <c r="F113" t="n">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="G113" t="n">
-        <v>0.4246469438076019</v>
+        <v>0.7144461870193481</v>
       </c>
       <c r="H113" t="inlineStr">
         <is>
-          <t>Tópico 8: crop, soil, tomato</t>
+          <t>Tópico 5: crop, soil, system</t>
         </is>
       </c>
       <c r="I113" t="inlineStr">
@@ -5053,14 +5097,14 @@
         </is>
       </c>
       <c r="F114" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="G114" t="n">
-        <v>0.8838904500007629</v>
+        <v>0.8713313341140747</v>
       </c>
       <c r="H114" t="inlineStr">
         <is>
-          <t>Tópico 2: protein, effector, sequence</t>
+          <t>Tópico 3: protein, effector, sequence</t>
         </is>
       </c>
       <c r="I114" t="inlineStr">
@@ -5094,14 +5138,14 @@
         </is>
       </c>
       <c r="F115" t="n">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="G115" t="n">
-        <v>0.7526243925094604</v>
+        <v>0.9934973120689392</v>
       </c>
       <c r="H115" t="inlineStr">
         <is>
-          <t>Tópico 8: crop, soil, tomato</t>
+          <t>Tópico 5: crop, soil, system</t>
         </is>
       </c>
       <c r="I115" t="inlineStr">
@@ -5129,18 +5173,20 @@
       <c r="D116" t="n">
         <v>2022</v>
       </c>
-      <c r="E116" t="n">
+      <c r="E116" t="inlineStr">
+        <is>
+          <t>No especificado</t>
+        </is>
+      </c>
+      <c r="F116" t="n">
         <v>0</v>
       </c>
-      <c r="F116" t="n">
-        <v>5</v>
-      </c>
       <c r="G116" t="n">
-        <v>0.7078269124031067</v>
+        <v>0.5492375493049622</v>
       </c>
       <c r="H116" t="inlineStr">
         <is>
-          <t>Tópico 6: cassava, accuracy, feature</t>
+          <t>Tópico 1: cassava, blight, potato</t>
         </is>
       </c>
       <c r="I116" t="inlineStr">
@@ -5168,18 +5214,20 @@
       <c r="D117" t="n">
         <v>2022</v>
       </c>
-      <c r="E117" t="n">
+      <c r="E117" t="inlineStr">
+        <is>
+          <t>No especificado</t>
+        </is>
+      </c>
+      <c r="F117" t="n">
         <v>0</v>
       </c>
-      <c r="F117" t="n">
-        <v>5</v>
-      </c>
       <c r="G117" t="n">
-        <v>0.7184826731681824</v>
+        <v>0.7204647064208984</v>
       </c>
       <c r="H117" t="inlineStr">
         <is>
-          <t>Tópico 6: cassava, accuracy, feature</t>
+          <t>Tópico 1: cassava, blight, potato</t>
         </is>
       </c>
       <c r="I117" t="inlineStr">
@@ -5207,18 +5255,20 @@
       <c r="D118" t="n">
         <v>2022</v>
       </c>
-      <c r="E118" t="n">
+      <c r="E118" t="inlineStr">
+        <is>
+          <t>No especificado</t>
+        </is>
+      </c>
+      <c r="F118" t="n">
         <v>0</v>
       </c>
-      <c r="F118" t="n">
-        <v>5</v>
-      </c>
       <c r="G118" t="n">
-        <v>0.7731437683105469</v>
+        <v>0.7564964294433594</v>
       </c>
       <c r="H118" t="inlineStr">
         <is>
-          <t>Tópico 6: cassava, accuracy, feature</t>
+          <t>Tópico 1: cassava, blight, potato</t>
         </is>
       </c>
       <c r="I118" t="inlineStr">
@@ -5255,11 +5305,11 @@
         <v>5</v>
       </c>
       <c r="G119" t="n">
-        <v>0.7345374226570129</v>
+        <v>0.4259781837463379</v>
       </c>
       <c r="H119" t="inlineStr">
         <is>
-          <t>Tópico 6: cassava, accuracy, feature</t>
+          <t>Tópico 6: soybean, vegetable, learningbased</t>
         </is>
       </c>
       <c r="I119" t="inlineStr">
@@ -5287,18 +5337,20 @@
       <c r="D120" t="n">
         <v>2022</v>
       </c>
-      <c r="E120" t="n">
+      <c r="E120" t="inlineStr">
+        <is>
+          <t>No especificado</t>
+        </is>
+      </c>
+      <c r="F120" t="n">
         <v>0</v>
       </c>
-      <c r="F120" t="n">
-        <v>5</v>
-      </c>
       <c r="G120" t="n">
-        <v>0.7979023456573486</v>
+        <v>0.495625376701355</v>
       </c>
       <c r="H120" t="inlineStr">
         <is>
-          <t>Tópico 6: cassava, accuracy, feature</t>
+          <t>Tópico 1: cassava, blight, potato</t>
         </is>
       </c>
       <c r="I120" t="inlineStr">
@@ -5332,14 +5384,14 @@
         </is>
       </c>
       <c r="F121" t="n">
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="G121" t="n">
-        <v>0.3832952976226807</v>
+        <v>0.3966308832168579</v>
       </c>
       <c r="H121" t="inlineStr">
         <is>
-          <t>Tópico 6: cassava, accuracy, feature</t>
+          <t>Tópico 1: cassava, blight, potato</t>
         </is>
       </c>
       <c r="I121" t="inlineStr">
@@ -5373,14 +5425,14 @@
         </is>
       </c>
       <c r="F122" t="n">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="G122" t="n">
-        <v>0.4626276791095734</v>
+        <v>0.607199490070343</v>
       </c>
       <c r="H122" t="inlineStr">
         <is>
-          <t>Tópico 3: nitrogen, model, soil</t>
+          <t>Tópico 5: crop, soil, system</t>
         </is>
       </c>
       <c r="I122" t="inlineStr">
@@ -5414,14 +5466,14 @@
         </is>
       </c>
       <c r="F123" t="n">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="G123" t="n">
-        <v>0.4808257222175598</v>
+        <v>0.8716010451316833</v>
       </c>
       <c r="H123" t="inlineStr">
         <is>
-          <t>Tópico 5: protein, approach, performance</t>
+          <t>Tópico 3: protein, effector, sequence</t>
         </is>
       </c>
       <c r="I123" t="inlineStr">
@@ -5449,18 +5501,20 @@
       <c r="D124" t="n">
         <v>2022</v>
       </c>
-      <c r="E124" t="n">
+      <c r="E124" t="inlineStr">
+        <is>
+          <t>No especificado</t>
+        </is>
+      </c>
+      <c r="F124" t="n">
         <v>0</v>
       </c>
-      <c r="F124" t="n">
-        <v>5</v>
-      </c>
       <c r="G124" t="n">
-        <v>0.8888351917266846</v>
+        <v>0.5131650567054749</v>
       </c>
       <c r="H124" t="inlineStr">
         <is>
-          <t>Tópico 6: cassava, accuracy, feature</t>
+          <t>Tópico 1: cassava, blight, potato</t>
         </is>
       </c>
       <c r="I124" t="inlineStr">
@@ -5494,14 +5548,14 @@
         </is>
       </c>
       <c r="F125" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="G125" t="n">
-        <v>0.6549259424209595</v>
+        <v>0.4154699444770813</v>
       </c>
       <c r="H125" t="inlineStr">
         <is>
-          <t>Tópico 8: crop, soil, tomato</t>
+          <t>Tópico 7: model, data, study</t>
         </is>
       </c>
       <c r="I125" t="inlineStr">
@@ -5529,18 +5583,20 @@
       <c r="D126" t="n">
         <v>2022</v>
       </c>
-      <c r="E126" t="n">
-        <v>0</v>
+      <c r="E126" t="inlineStr">
+        <is>
+          <t>No especificado</t>
+        </is>
       </c>
       <c r="F126" t="n">
-        <v>7</v>
+        <v>1</v>
       </c>
       <c r="G126" t="n">
-        <v>0.8511449694633484</v>
+        <v>0.6953845620155334</v>
       </c>
       <c r="H126" t="inlineStr">
         <is>
-          <t>Tópico 8: crop, soil, tomato</t>
+          <t>Tópico 2: tomato, fruit, grape</t>
         </is>
       </c>
       <c r="I126" t="inlineStr">
@@ -5574,14 +5630,14 @@
         </is>
       </c>
       <c r="F127" t="n">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="G127" t="n">
-        <v>0.9088655114173889</v>
+        <v>0.5760210156440735</v>
       </c>
       <c r="H127" t="inlineStr">
         <is>
-          <t>Tópico 6: cassava, accuracy, feature</t>
+          <t>Tópico 7: model, data, study</t>
         </is>
       </c>
       <c r="I127" t="inlineStr">
@@ -5615,14 +5671,14 @@
         </is>
       </c>
       <c r="F128" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="G128" t="n">
-        <v>0.6451596617698669</v>
+        <v>0.5894243121147156</v>
       </c>
       <c r="H128" t="inlineStr">
         <is>
-          <t>Tópico 8: crop, soil, tomato</t>
+          <t>Tópico 7: model, data, study</t>
         </is>
       </c>
       <c r="I128" t="inlineStr">
@@ -5656,14 +5712,14 @@
         </is>
       </c>
       <c r="F129" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="G129" t="n">
-        <v>0.5491819381713867</v>
+        <v>0.6878044009208679</v>
       </c>
       <c r="H129" t="inlineStr">
         <is>
-          <t>Tópico 2: protein, effector, sequence</t>
+          <t>Tópico 3: protein, effector, sequence</t>
         </is>
       </c>
       <c r="I129" t="inlineStr">
@@ -5697,14 +5753,14 @@
         </is>
       </c>
       <c r="F130" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="G130" t="n">
-        <v>0.9109036326408386</v>
+        <v>0.9220969080924988</v>
       </c>
       <c r="H130" t="inlineStr">
         <is>
-          <t>Tópico 2: protein, effector, sequence</t>
+          <t>Tópico 3: protein, effector, sequence</t>
         </is>
       </c>
       <c r="I130" t="inlineStr">
@@ -5738,14 +5794,14 @@
         </is>
       </c>
       <c r="F131" t="n">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="G131" t="n">
-        <v>0.7039441466331482</v>
+        <v>0.9884282350540161</v>
       </c>
       <c r="H131" t="inlineStr">
         <is>
-          <t>Tópico 5: protein, approach, performance</t>
+          <t>Tópico 3: protein, effector, sequence</t>
         </is>
       </c>
       <c r="I131" t="inlineStr">
@@ -5779,14 +5835,14 @@
         </is>
       </c>
       <c r="F132" t="n">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="G132" t="n">
-        <v>0.4824055731296539</v>
+        <v>0.3617160618305206</v>
       </c>
       <c r="H132" t="inlineStr">
         <is>
-          <t>Tópico 8: crop, soil, tomato</t>
+          <t>Tópico 6: soybean, vegetable, learningbased</t>
         </is>
       </c>
       <c r="I132" t="inlineStr">
@@ -5823,11 +5879,11 @@
         <v>0</v>
       </c>
       <c r="G133" t="n">
-        <v>0.3711137473583221</v>
+        <v>0.358305037021637</v>
       </c>
       <c r="H133" t="inlineStr">
         <is>
-          <t>Tópico 1: model, nitrogen, network</t>
+          <t>Tópico 1: cassava, blight, potato</t>
         </is>
       </c>
       <c r="I133" t="inlineStr">
@@ -5861,14 +5917,14 @@
         </is>
       </c>
       <c r="F134" t="n">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="G134" t="n">
-        <v>0.4921607077121735</v>
+        <v>0.5780991911888123</v>
       </c>
       <c r="H134" t="inlineStr">
         <is>
-          <t>Tópico 3: nitrogen, model, soil</t>
+          <t>Tópico 5: crop, soil, system</t>
         </is>
       </c>
       <c r="I134" t="inlineStr">
@@ -5896,18 +5952,20 @@
       <c r="D135" t="n">
         <v>2021</v>
       </c>
-      <c r="E135" t="n">
-        <v>0</v>
+      <c r="E135" t="inlineStr">
+        <is>
+          <t>No especificado</t>
+        </is>
       </c>
       <c r="F135" t="n">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="G135" t="n">
-        <v>0.6476060152053833</v>
+        <v>0.5713438391685486</v>
       </c>
       <c r="H135" t="inlineStr">
         <is>
-          <t>Tópico 6: cassava, accuracy, feature</t>
+          <t>Tópico 2: tomato, fruit, grape</t>
         </is>
       </c>
       <c r="I135" t="inlineStr">
@@ -5935,18 +5993,20 @@
       <c r="D136" t="n">
         <v>2021</v>
       </c>
-      <c r="E136" t="n">
-        <v>0</v>
+      <c r="E136" t="inlineStr">
+        <is>
+          <t>No especificado</t>
+        </is>
       </c>
       <c r="F136" t="n">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="G136" t="n">
-        <v>0.6796565055847168</v>
+        <v>0.712571918964386</v>
       </c>
       <c r="H136" t="inlineStr">
         <is>
-          <t>Tópico 8: crop, soil, tomato</t>
+          <t>Tópico 5: crop, soil, system</t>
         </is>
       </c>
       <c r="I136" t="inlineStr">
@@ -5980,14 +6040,14 @@
         </is>
       </c>
       <c r="F137" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="G137" t="n">
-        <v>0.5329149961471558</v>
+        <v>0.4024023711681366</v>
       </c>
       <c r="H137" t="inlineStr">
         <is>
-          <t>Tópico 6: cassava, accuracy, feature</t>
+          <t>Tópico 5: crop, soil, system</t>
         </is>
       </c>
       <c r="I137" t="inlineStr">
@@ -6021,14 +6081,14 @@
         </is>
       </c>
       <c r="F138" t="n">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="G138" t="n">
-        <v>0.8972112536430359</v>
+        <v>0.5912401080131531</v>
       </c>
       <c r="H138" t="inlineStr">
         <is>
-          <t>Tópico 8: crop, soil, tomato</t>
+          <t>Tópico 5: crop, soil, system</t>
         </is>
       </c>
       <c r="I138" t="inlineStr">
@@ -6062,14 +6122,14 @@
         </is>
       </c>
       <c r="F139" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="G139" t="n">
-        <v>0.3193668127059937</v>
+        <v>0.8651778101921082</v>
       </c>
       <c r="H139" t="inlineStr">
         <is>
-          <t>Tópico 6: cassava, accuracy, feature</t>
+          <t>Tópico 5: crop, soil, system</t>
         </is>
       </c>
       <c r="I139" t="inlineStr">
@@ -6103,14 +6163,14 @@
         </is>
       </c>
       <c r="F140" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="G140" t="n">
-        <v>0.8722729682922363</v>
+        <v>0.9772552847862244</v>
       </c>
       <c r="H140" t="inlineStr">
         <is>
-          <t>Tópico 2: protein, effector, sequence</t>
+          <t>Tópico 3: protein, effector, sequence</t>
         </is>
       </c>
       <c r="I140" t="inlineStr">
@@ -6144,14 +6204,14 @@
         </is>
       </c>
       <c r="F141" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="G141" t="n">
-        <v>0.342653751373291</v>
+        <v>0.8838339447975159</v>
       </c>
       <c r="H141" t="inlineStr">
         <is>
-          <t>Tópico 1: model, nitrogen, network</t>
+          <t>Tópico 3: protein, effector, sequence</t>
         </is>
       </c>
       <c r="I141" t="inlineStr">
@@ -6185,14 +6245,14 @@
         </is>
       </c>
       <c r="F142" t="n">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="G142" t="n">
-        <v>0.752605140209198</v>
+        <v>0.6254897713661194</v>
       </c>
       <c r="H142" t="inlineStr">
         <is>
-          <t>Tópico 6: cassava, accuracy, feature</t>
+          <t>Tópico 2: tomato, fruit, grape</t>
         </is>
       </c>
       <c r="I142" t="inlineStr">
@@ -6226,14 +6286,14 @@
         </is>
       </c>
       <c r="F143" t="n">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="G143" t="n">
-        <v>0.4839813113212585</v>
+        <v>0.782441258430481</v>
       </c>
       <c r="H143" t="inlineStr">
         <is>
-          <t>Tópico 3: nitrogen, model, soil</t>
+          <t>Tópico 5: crop, soil, system</t>
         </is>
       </c>
       <c r="I143" t="inlineStr">
@@ -6267,14 +6327,14 @@
         </is>
       </c>
       <c r="F144" t="n">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="G144" t="n">
-        <v>0.5620536208152771</v>
+        <v>0.4902197122573853</v>
       </c>
       <c r="H144" t="inlineStr">
         <is>
-          <t>Tópico 6: cassava, accuracy, feature</t>
+          <t>Tópico 2: tomato, fruit, grape</t>
         </is>
       </c>
       <c r="I144" t="inlineStr">
@@ -6308,14 +6368,14 @@
         </is>
       </c>
       <c r="F145" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="G145" t="n">
-        <v>0.6881983876228333</v>
+        <v>0.5852974057197571</v>
       </c>
       <c r="H145" t="inlineStr">
         <is>
-          <t>Tópico 8: crop, soil, tomato</t>
+          <t>Tópico 7: model, data, study</t>
         </is>
       </c>
       <c r="I145" t="inlineStr">
@@ -6349,14 +6409,14 @@
         </is>
       </c>
       <c r="F146" t="n">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="G146" t="n">
-        <v>0.7718408107757568</v>
+        <v>0.9923004508018494</v>
       </c>
       <c r="H146" t="inlineStr">
         <is>
-          <t>Tópico 5: protein, approach, performance</t>
+          <t>Tópico 3: protein, effector, sequence</t>
         </is>
       </c>
       <c r="I146" t="inlineStr">
@@ -6390,14 +6450,14 @@
         </is>
       </c>
       <c r="F147" t="n">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="G147" t="n">
-        <v>0.5134264826774597</v>
+        <v>0.4417244791984558</v>
       </c>
       <c r="H147" t="inlineStr">
         <is>
-          <t>Tópico 8: crop, soil, tomato</t>
+          <t>Tópico 6: soybean, vegetable, learningbased</t>
         </is>
       </c>
       <c r="I147" t="inlineStr">
@@ -6431,14 +6491,14 @@
         </is>
       </c>
       <c r="F148" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="G148" t="n">
-        <v>0.8108813166618347</v>
+        <v>0.986865222454071</v>
       </c>
       <c r="H148" t="inlineStr">
         <is>
-          <t>Tópico 2: protein, effector, sequence</t>
+          <t>Tópico 3: protein, effector, sequence</t>
         </is>
       </c>
       <c r="I148" t="inlineStr">
@@ -6466,18 +6526,20 @@
       <c r="D149" t="n">
         <v>2018</v>
       </c>
-      <c r="E149" t="n">
-        <v>0</v>
+      <c r="E149" t="inlineStr">
+        <is>
+          <t>No especificado</t>
+        </is>
       </c>
       <c r="F149" t="n">
-        <v>7</v>
+        <v>1</v>
       </c>
       <c r="G149" t="n">
-        <v>0.8761871457099915</v>
+        <v>0.5071201324462891</v>
       </c>
       <c r="H149" t="inlineStr">
         <is>
-          <t>Tópico 8: crop, soil, tomato</t>
+          <t>Tópico 2: tomato, fruit, grape</t>
         </is>
       </c>
       <c r="I149" t="inlineStr">
@@ -6511,14 +6573,14 @@
         </is>
       </c>
       <c r="F150" t="n">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="G150" t="n">
-        <v>0.5879806280136108</v>
+        <v>0.5320999026298523</v>
       </c>
       <c r="H150" t="inlineStr">
         <is>
-          <t>Tópico 3: nitrogen, model, soil</t>
+          <t>Tópico 6: soybean, vegetable, learningbased</t>
         </is>
       </c>
       <c r="I150" t="inlineStr">
@@ -6546,18 +6608,20 @@
       <c r="D151" t="n">
         <v>2017</v>
       </c>
-      <c r="E151" t="n">
-        <v>0</v>
+      <c r="E151" t="inlineStr">
+        <is>
+          <t>No especificado</t>
+        </is>
       </c>
       <c r="F151" t="n">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="G151" t="n">
-        <v>0.69129478931427</v>
+        <v>0.5773987770080566</v>
       </c>
       <c r="H151" t="inlineStr">
         <is>
-          <t>Tópico 6: cassava, accuracy, feature</t>
+          <t>Tópico 2: tomato, fruit, grape</t>
         </is>
       </c>
       <c r="I151" t="inlineStr">
@@ -6591,14 +6655,14 @@
         </is>
       </c>
       <c r="F152" t="n">
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="G152" t="n">
-        <v>0.8923659324645996</v>
+        <v>0.9908394813537598</v>
       </c>
       <c r="H152" t="inlineStr">
         <is>
-          <t>Tópico 6: cassava, accuracy, feature</t>
+          <t>Tópico 1: cassava, blight, potato</t>
         </is>
       </c>
       <c r="I152" t="inlineStr">
@@ -6632,14 +6696,14 @@
         </is>
       </c>
       <c r="F153" t="n">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="G153" t="n">
-        <v>0.4507667422294617</v>
+        <v>0.7331138849258423</v>
       </c>
       <c r="H153" t="inlineStr">
         <is>
-          <t>Tópico 5: protein, approach, performance</t>
+          <t>Tópico 3: protein, effector, sequence</t>
         </is>
       </c>
       <c r="I153" t="inlineStr">
@@ -6673,14 +6737,14 @@
         </is>
       </c>
       <c r="F154" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="G154" t="n">
-        <v>0.581308126449585</v>
+        <v>0.6445139646530151</v>
       </c>
       <c r="H154" t="inlineStr">
         <is>
-          <t>Tópico 2: protein, effector, sequence</t>
+          <t>Tópico 3: protein, effector, sequence</t>
         </is>
       </c>
       <c r="I154" t="inlineStr">
@@ -6714,14 +6778,14 @@
         </is>
       </c>
       <c r="F155" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="G155" t="n">
-        <v>0.6093983054161072</v>
+        <v>0.7025050520896912</v>
       </c>
       <c r="H155" t="inlineStr">
         <is>
-          <t>Tópico 4: gene, bacterial, target</t>
+          <t>Tópico 3: protein, effector, sequence</t>
         </is>
       </c>
       <c r="I155" t="inlineStr">
@@ -6749,18 +6813,20 @@
       <c r="D156" t="n">
         <v>2013</v>
       </c>
-      <c r="E156" t="n">
-        <v>0</v>
+      <c r="E156" t="inlineStr">
+        <is>
+          <t>No especificado</t>
+        </is>
       </c>
       <c r="F156" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="G156" t="n">
-        <v>0.5917408466339111</v>
+        <v>0.6064732670783997</v>
       </c>
       <c r="H156" t="inlineStr">
         <is>
-          <t>Tópico 2: protein, effector, sequence</t>
+          <t>Tópico 3: protein, effector, sequence</t>
         </is>
       </c>
       <c r="I156" t="inlineStr">
@@ -6772,673 +6838,669 @@
     <row r="157">
       <c r="A157" t="inlineStr">
         <is>
-          <t>10.3390/electronics12122706</t>
+          <t>10.1109/MVIP62238.2024.10491178</t>
         </is>
       </c>
       <c r="B157" t="inlineStr">
         <is>
-          <t>Attention mechanisms in convolutional neural networks for nitrogen treatment detection in tomato leaves using hyperspectral images</t>
+          <t>Tomato Leaf Disease Detection Using Transfer Learning: A Comparative Study</t>
         </is>
       </c>
       <c r="C157" t="inlineStr">
         <is>
-          <t>['B Benmouna', 'R Pourdarbani', 'S Sabzi']</t>
+          <t>M. Bahrami; A. Pourhatami; M. Maboodi</t>
         </is>
       </c>
       <c r="D157" t="n">
-        <v>2023</v>
+        <v>2024</v>
       </c>
       <c r="E157" t="inlineStr">
         <is>
-          <t>Electronics</t>
+          <t>2024 13th Iranian/3rd International Machine Vision and Image Processing Conference (MVIP)</t>
         </is>
       </c>
       <c r="F157" t="n">
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="G157" t="n">
-        <v>0.7495788931846619</v>
+        <v>0.697862982749939</v>
       </c>
       <c r="H157" t="inlineStr">
         <is>
-          <t>Tópico 1: model, nitrogen, network</t>
+          <t>Tópico 7: model, data, study</t>
         </is>
       </c>
       <c r="I157" t="inlineStr">
         <is>
-          <t>studies to estimate the amount of nitrogen in plant leaves. In  on deep learning and  convolutional neural networks are able  nitrogen in plants but to detect the misapplication of</t>
+          <t>Tomato, a vital food crop enriched with essential minerals and vitamins, is widely used in various cuisines. Leaf disease is a common problem that significantly impacts the quantity and quality of tomato production. So, farmers should accurately surveil tomato farms to manufacture high-quality foods free from pests. In this regard, accurate and robust algorithms are needed to detect tomato leaf disease. Among various methods, deep learning algorithms provide automatic, accurate, and robust leaf disease detection algorithms. In this paper, a comprehensive analysis of different transfer learning algorithms, including VGG19, ResNet-101, and MobileNet-v2 was done on PlantVillage and CCMT datasets. The best performance was achieved by VGG19, where the best accuracy, precision, recall, and F1-score on the test set of PlantVillage and CCMT datasets were 99.48%, 99.27%, 99.28%, 99.27%, and 92.76%, 92.74%, 95.09%, 90.86%, respectively. The results demonstrate that VGG19 can detect tomato leaf disease precisely and robustly.</t>
         </is>
       </c>
     </row>
     <row r="158">
       <c r="A158" t="inlineStr">
         <is>
-          <t>10.1016/s0169-5347(99)01596-7</t>
+          <t>10.1109/ICOSEC61587.2024.10722678</t>
         </is>
       </c>
       <c r="B158" t="inlineStr">
         <is>
-          <t>… of recent research in the United States on the role of freshwater and saltwater wetlands as sources, sinks, and transformers of nitrogen, phosphorus, and various …</t>
+          <t>A Detailed Investigation of Deep Learning and Machine Learning Approaches for Sugarcane Foliage Disorder Identification</t>
         </is>
       </c>
       <c r="C158" t="inlineStr">
         <is>
-          <t>['SW Nixon', 'V Lee']</t>
+          <t>R. T. Khatoon; D. Ashok; S. K. R. Mallidi; V. Gopikrishna; P. Srikanth; P. Bhaskar</t>
         </is>
       </c>
       <c r="D158" t="n">
-        <v>1986</v>
+        <v>2024</v>
       </c>
       <c r="E158" t="inlineStr">
         <is>
-          <t>NA</t>
+          <t>2024 5th International Conference on Smart Electronics and Communication (ICOSEC)</t>
         </is>
       </c>
       <c r="F158" t="n">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="G158" t="n">
-        <v>0.960566520690918</v>
+        <v>0.598248302936554</v>
       </c>
       <c r="H158" t="inlineStr">
         <is>
-          <t>Tópico 3: nitrogen, model, soil</t>
+          <t>Tópico 5: crop, soil, system</t>
         </is>
       </c>
       <c r="I158" t="inlineStr">
         <is>
-          <t>The coterminous United States and Alaska were divided into seven geographic regions  representing groups of Corps of Engineers Districts. Within each geographic region, the quality</t>
+          <t>Our nation grows an enormous amount of sugarcane. Sugarcane is no exception to the rule that plants are susceptible to disease. One problem with the sugar industry is that small-scale farmers lose revenue when sugarcane diseases aren’t identified and addressed in time to save the growing crops. A popular way for a farmer to discover and diagnose sugarcane illnesses is by visual inspection. Using this method on large farms becomes more laborious and time-consuming. The farmers and sugarcane business are both put at risk if it is not handled sooner. This inquiry was motivated by the ever-increasing types of ailments and the fact that farmers have limited abilities when it comes to diagnosing and identifying these diseases. A combination of Deep Learning (DL), Computer Vision (CV), and Machine Learning (ML) can solve this challenge. To boost agricultural output and efficiency, specialists have taken an interest in prompt disease identification and diagnosis. Losses may be avoided by employing ML and DL algorithms for early disease detection in sugarcane crops. The purpose of this research was to quickly and accurately extract diagnostic information from sugarcane using a variety of image processing and DL methods. Additionally, the difficulties and potential future directions of computational methods for evaluating sugarcane infestations are brought to light.</t>
         </is>
       </c>
     </row>
     <row r="159">
       <c r="A159" t="inlineStr">
         <is>
-          <t>10.1039/d5qm00140d</t>
+          <t>10.1109/ICMLC.2010.21</t>
         </is>
       </c>
       <c r="B159" t="inlineStr">
         <is>
-          <t>Machine-learning enables nitrogen reduction reaction on transition metal doped C 3 B by controlling the charge states</t>
+          <t>SVM Model for Amino Acid Composition Based Prediction of MMPs and ADAMs</t>
         </is>
       </c>
       <c r="C159" t="inlineStr">
         <is>
-          <t>['C Yang', 'C Yang', 'Y Liang', 'H Yan', 'A Zhang']</t>
+          <t>K. Pant; B. Pant; K. R. Pardasani</t>
         </is>
       </c>
       <c r="D159" t="n">
-        <v>2025</v>
+        <v>2010</v>
       </c>
       <c r="E159" t="inlineStr">
         <is>
-          <t>Materials Chemistry …</t>
+          <t>2010 Second International Conference on Machine Learning and Computing</t>
         </is>
       </c>
       <c r="F159" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="G159" t="n">
-        <v>0.4953416287899017</v>
+        <v>0.7592259049415588</v>
       </c>
       <c r="H159" t="inlineStr">
         <is>
-          <t>Tópico 2: protein, effector, sequence</t>
+          <t>Tópico 3: protein, effector, sequence</t>
         </is>
       </c>
       <c r="I159" t="inlineStr">
         <is>
-          <t>Nevertheless, developing efficient nitrogen reduction reaction (NRR)  machine learning  (ML) revealed that the number of TM valence electrons and the presence of nitrogen substituents</t>
+          <t>The MMPs and ADAMs are cell surface proteases which belong to metalloprotease family. They play an important role in skin aging, skin disorders, anticancer therapy and other physiological disorders. Thus there arises the need to understand the relationships among various parameters of these proteins for prediction of their classes, structures and functionality. The computational approaches for prediction of their classes are fast and economical therefore can be used to complement the existing wet lab techniques. Realizing their importance, in this paper an attempt has been made to correlate them with their amino acid composition and predict them with fair accuracy. This is a novel method where ADAMs and MMPs have been classified on the basis of amino acid composition using Support Vector Machine. The SVM has been implemented using Lib SVM package. The method discriminates MMP subfamily from ADAM proteases with Matthew's correlation coefficient of 0.98 using amino acid composition. The performance of the method was evaluated using 5-fold cross-validation where accuracy of 98% was obtained.</t>
         </is>
       </c>
     </row>
     <row r="160">
       <c r="A160" t="inlineStr">
         <is>
-          <t>10.1039/d4tc05271d</t>
+          <t>10.1109/AECE59614.2023.10428363</t>
         </is>
       </c>
       <c r="B160" t="inlineStr">
         <is>
-          <t>Designing a machine learning-optimized nitrogen and sulfur co-doped CoNi@ SiO 2 electrocatalyst for high performance oxygen evolution reaction</t>
+          <t>A Novel Cloud-Based Framework for Leaf Disease Detection and Classification: Enhancing Plant Health Using Android Applications</t>
         </is>
       </c>
       <c r="C160" t="inlineStr">
         <is>
-          <t>['M Waseem', 'SM El-Bahy', 'MMH Maqbool']</t>
+          <t>A. Kiran; A. Namdev; R. R. Chandan; P. B. Waghmare; D. Dhabliya; A. Gupta</t>
         </is>
       </c>
       <c r="D160" t="n">
-        <v>2025</v>
+        <v>2023</v>
       </c>
       <c r="E160" t="inlineStr">
         <is>
-          <t>Journal of Materials …</t>
+          <t>2023 3rd International Conference on Advancement in Electronics &amp; Communication Engineering (AECE)</t>
         </is>
       </c>
       <c r="F160" t="n">
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="G160" t="n">
-        <v>0.5287150144577026</v>
+        <v>0.4900111854076385</v>
       </c>
       <c r="H160" t="inlineStr">
         <is>
-          <t>Tópico 1: model, nitrogen, network</t>
+          <t>Tópico 7: model, data, study</t>
         </is>
       </c>
       <c r="I160" t="inlineStr">
         <is>
-          <t>Although various heteroatom-doped bimetallic composites have been explored for the oxygen  evolution reaction (OER), they often suffer from aggregation and low electrical conductivity</t>
+          <t>The difficult challenge of identifying the leaf disease in agriculture is employed to stop the dangerous epidemic. The majority of plant diseases are brought on by fungus, bacteria, and viruses, with the fungi often attached to the plant's reproductive organs. As a result, bacteria have simpler life cycles and are more dangerous than fungi. Similar to bacteria, viruses are microscopic particles that contain genetic information and protein but no additional protein. Therefore, it is crucial to spot illness in plant leaves. Therefore, the goal of this research is to identify leaf disease in a cloudy environment. The use of smartphones for many applications has increased recently. A brand-new operating system called Android is freely accessible in the Android Market. Thus, this study uses an Android application to develop a cloud-based illness categorization system.</t>
         </is>
       </c>
     </row>
     <row r="161">
       <c r="A161" t="inlineStr">
         <is>
-          <t>10.3390/pr12061167</t>
+          <t>10.1109/PDGC56933.2022.10053320</t>
         </is>
       </c>
       <c r="B161" t="inlineStr">
         <is>
-          <t>Pressure Characteristics in the Nitrogen-Sealed Power Transformers under Internal Faults</t>
+          <t>Analysis of Apple Plant Leaf Diseases Detection and Classification: A Review</t>
         </is>
       </c>
       <c r="C161" t="inlineStr">
         <is>
-          <t>['J Li', 'Z Jia', 'S Wang', 'S Liu']</t>
+          <t>S. Kumar; R. Kumar; M. Gupta</t>
         </is>
       </c>
       <c r="D161" t="n">
-        <v>2024</v>
+        <v>2022</v>
       </c>
       <c r="E161" t="inlineStr">
         <is>
-          <t>Processes</t>
+          <t>2022 Seventh International Conference on Parallel, Distributed and Grid Computing (PDGC)</t>
         </is>
       </c>
       <c r="F161" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="G161" t="n">
-        <v>0.8439958095550537</v>
+        <v>0.5088988542556763</v>
       </c>
       <c r="H161" t="inlineStr">
         <is>
-          <t>Tópico 3: nitrogen, model, soil</t>
+          <t>Tópico 2: tomato, fruit, grape</t>
         </is>
       </c>
       <c r="I161" t="inlineStr">
         <is>
-          <t>The explosion-proof performance is an important index for oil-immersed transformers. The  nitrogen-sealed transformer is a new type of transformer with nitrogen gas in the upper space,</t>
+          <t>Agriculture has a vital role in the development of any country like India where the majority of the population’s livelihood depends on agriculture. Every year, diseases and pests harm apple production by a significant amount of money. Farmers face a challenge in identifying distinct apple illnesses because the symptoms of different illnesses can be extremely similar and occur at the same time. Therefore, Leaf Disease Prediction (LDP) in apple cultivation is considerably important to overcome these problems. In this work, an overview of the taxonomy of apple plant diseases is discussed with their symptoms, cause, and effect. This study concluded that the method used for automatic detection and classification of apple plant diseases is still in its infancy. Hence, a new efficient model is required for the detection and classification of apple plant leaf disease that can save the farmer from loss as well as help them in increasing the production of apples.</t>
         </is>
       </c>
     </row>
     <row r="162">
       <c r="A162" t="inlineStr">
         <is>
-          <t>10.1016/j.compag.2018.05.012</t>
+          <t>10.1109/ICET54505.2021.9689807</t>
         </is>
       </c>
       <c r="B162" t="inlineStr">
         <is>
-          <t>Machine learning approaches for crop yield prediction and nitrogen status estimation in precision agriculture: A review</t>
+          <t>Identification of Leaf Diseases in Potato Crop Using Deep Convolutional Neural Networks (DCNNs)</t>
         </is>
       </c>
       <c r="C162" t="inlineStr">
         <is>
-          <t>['A Chlingaryan', 'S Sukkarieh', 'B Whelan']</t>
+          <t>Z. Saeed; M. Urooj Khan; A. Raza; N. Sajjad; S. Naz; A. Salal</t>
         </is>
       </c>
       <c r="D162" t="n">
-        <v>2018</v>
+        <v>2021</v>
       </c>
       <c r="E162" t="inlineStr">
         <is>
-          <t>Computers and electronics in …</t>
+          <t>2021 16th International Conference on Emerging Technologies (ICET)</t>
         </is>
       </c>
       <c r="F162" t="n">
-        <v>7</v>
+        <v>0</v>
       </c>
       <c r="G162" t="n">
-        <v>0.5663738250732422</v>
+        <v>0.5312085151672363</v>
       </c>
       <c r="H162" t="inlineStr">
         <is>
-          <t>Tópico 8: crop, soil, tomato</t>
+          <t>Tópico 1: cassava, blight, potato</t>
         </is>
       </c>
       <c r="I162" t="inlineStr">
         <is>
-          <t>This is due to the capability of machine learning based systems to process a large number   on machine learning based techniques for accurate crop yield prediction and nitrogen status</t>
+          <t>Potatoes are used by a billion people globally as its intake per capita is 31.3 kilograms per month worldwide and its crop production surpasses 300 million metric tons. They have great nutritional potential and offer more protein and iron than other vegetables. Various diseases, such as early blight, late blight, and others, will attack potato plants and manifest their symptoms in the leaves. If these outbreaks are discovered early and appropriate treatment is taken, the farmer will not suffer significant economic losses. In this article, the suggested computer vision deep learning approach would significantly help in early identification and detection of different potato disease. Many plant diseases have different visual characteristics that may be utilized to accurately identify and classify them. This study describes a potato disease classification method based on computer vision-deep learning combination. The system trains deep convolutional neural networks such as ResNet-152 and InceptionV3 on the Kaggle potato dataset with an accuracy of 98.34% and 95.24% respectively at learning rate of 0.0005. This system successfully performs the classification of three categories: healthy, early, and late blight for potato leaves.</t>
         </is>
       </c>
     </row>
     <row r="163">
       <c r="A163" t="inlineStr">
         <is>
-          <t>10.1016/j.envint.2019.104934</t>
+          <t>10.1109/ACCESS.2024.3407153</t>
         </is>
       </c>
       <c r="B163" t="inlineStr">
         <is>
-          <t>A comparison of linear regression, regularization, and machine learning algorithms to develop Europe-wide spatial models of fine particles and nitrogen dioxide</t>
+          <t>Mulberry Leaf Disease Detection Using CNN-Based Smart Android Application</t>
         </is>
       </c>
       <c r="C163" t="inlineStr">
         <is>
-          <t>['J Chen', 'K de Hoogh', 'J Gulliver', 'B Hoffmann']</t>
+          <t>A. Salam; M. Naznine; N. Jahan; E. Nahid; M. Nahiduzzaman; M. E. H. Chowdhury</t>
         </is>
       </c>
       <c r="D163" t="n">
-        <v>2019</v>
+        <v>2024</v>
       </c>
       <c r="E163" t="inlineStr">
         <is>
-          <t>Environment …</t>
+          <t>IEEE Access</t>
         </is>
       </c>
       <c r="F163" t="n">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="G163" t="n">
-        <v>0.631507933139801</v>
+        <v>0.5830755233764648</v>
       </c>
       <c r="H163" t="inlineStr">
         <is>
-          <t>Tópico 1: model, nitrogen, network</t>
+          <t>Tópico 5: crop, soil, system</t>
         </is>
       </c>
       <c r="I163" t="inlineStr">
         <is>
-          <t>) and nitrogen dioxide (NO 2 ) concentrations across Europe. The evaluated algorithms  included linear stepwise regression, regularization techniques and machine learning methods.</t>
+          <t>Mulberry leaves serve as the primary food source for Bombyx mori silkworms, crucial for silk thread production. However, mulberry trees are highly susceptible to diseases, spreading rapidly and causing significant losses. Manual disease identification across large farms is arduous and time-consuming. Leveraging computer vision for early disease detection and classification can mitigate up to 90% of production losses. This study collected leaves from two regions of Bangladesh, categorized as healthy, leaf rust-affected, and leaf spot-affected. With a total of 1091 images, split into training (764), testing (218), and validation (109) sets for 5-fold cross-validation, preprocessing and augmentation yielded 6,000 images, including synthetics. This study compares ResNet50, VGG19, and MobileNetV3Small on a specific task following architecture modifications. Four convolutional layers with different output channels (512, 128, 64, and 32) were added to baseline models. We assessed how these architectural changes affected model correctness, computing efficiency, and convergence rates. Comparing three pretrained convolutional neural networks (CNNs) - MobileNetV3Small, ResNet50, and VGG19 - augmented with four additional layers, the modified MobileNetV3Small excelled in precision, recall, F1-score, and accuracy, achieving notable results of 97.0%, 96.4%, 96.4%, and 96.4%, respectively, across cross-validation folds. An efficient smartphone application employing the proposed model for mulberry leaf disease recognition was developed. Overall, the model outperformed existing State of the Art (SOTA) approaches, showcasing its effectiveness in disease identification. The interpretative Grad-CAM visualization images match sericulture specialists’ assessments, validating the model’s predictions. These results imply that, this eXplainable AI (XAI) approach with a modified deep learning architecture can appropriately classify mulberry leaves.</t>
         </is>
       </c>
     </row>
     <row r="164">
       <c r="A164" t="inlineStr">
         <is>
-          <t>10.5391/ijfis.2021.21.1.1</t>
+          <t>10.1109/ICEET56468.2022.10007133</t>
         </is>
       </c>
       <c r="B164" t="inlineStr">
         <is>
-          <t>Rice fungal diseases recognition using modern computer vision techniques</t>
+          <t>Federated learning-based UAVs for the diagnosis of Plant Diseases</t>
         </is>
       </c>
       <c r="C164" t="inlineStr">
         <is>
-          <t>['IV Arinichev', 'SV Polyanskikh', 'GV Volkova']</t>
+          <t>F. S. Khan; S. Khan; M. N. H. Mohd; A. Waseem; M. N. A. Khan; S. Ali; R. Ahmed</t>
         </is>
       </c>
       <c r="D164" t="n">
-        <v>2021</v>
+        <v>2022</v>
       </c>
       <c r="E164" t="inlineStr">
         <is>
-          <t>International Journal of …</t>
+          <t>2022 International Conference on Engineering and Emerging Technologies (ICEET)</t>
         </is>
       </c>
       <c r="F164" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="G164" t="n">
-        <v>0.5607926249504089</v>
+        <v>0.7798483371734619</v>
       </c>
       <c r="H164" t="inlineStr">
         <is>
-          <t>Tópico 6: cassava, accuracy, feature</t>
+          <t>Tópico 5: crop, soil, system</t>
         </is>
       </c>
       <c r="I164" t="inlineStr">
         <is>
-          <t>some fungal diseases of rice using visual computing and machine learning techniques. Leaf  blast and brown spot diseases are considered. Modern computer vision methods based on</t>
+          <t>The technological revolution for farmers, especially for the safety of their crops from pests, plays an evident change and convenience for the agriculture industry. The current research presented the classification of different pests using federated learning-based UAVs. The designed scenarios comprise four different sites connected with a global model where different parameters for these sites are received from the local model. State-of-the-art EfficientNet deep model with B03 configurations provides the best accuracy for classifying nine types of pests. The system can achieve an accuracy of 99.55% with the augmentation of images into different angles. The federated learning designed UAVs are the most reliable connection with very less computation power during the classification of pests for the agricultural environment.</t>
         </is>
       </c>
     </row>
     <row r="165">
       <c r="A165" t="inlineStr">
         <is>
-          <t>10.1016/j.biosystemseng.2016.04.018</t>
+          <t>10.1109/INCET64471.2025.11140131</t>
         </is>
       </c>
       <c r="B165" t="inlineStr">
         <is>
-          <t>Machine learning based prediction of soil total nitrogen, organic carbon and moisture content by using VIS-NIR spectroscopy</t>
+          <t>Tomato Leaf Disease Detection Using a Convolutional Neural Network</t>
         </is>
       </c>
       <c r="C165" t="inlineStr">
         <is>
-          <t>['A Morellos', 'XE Pantazi', 'D Moshou', 'T Alexandridis']</t>
+          <t>K. K. Kumar; R. Jawwharlal; V. S; J. B. Naik; B. Suma; A. Gupta</t>
         </is>
       </c>
       <c r="D165" t="n">
-        <v>2016</v>
+        <v>2025</v>
       </c>
       <c r="E165" t="inlineStr">
         <is>
-          <t>Biosystems …</t>
+          <t>2025 6th International Conference for Emerging Technology (INCET)</t>
         </is>
       </c>
       <c r="F165" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G165" t="n">
-        <v>0.9665206074714661</v>
+        <v>0.7895268201828003</v>
       </c>
       <c r="H165" t="inlineStr">
         <is>
-          <t>Tópico 1: model, nitrogen, network</t>
+          <t>Tópico 2: tomato, fruit, grape</t>
         </is>
       </c>
       <c r="I165" t="inlineStr">
         <is>
-          <t>-NIR) spectroscopy has the potential of estimating soil total nitrogen (TN), organic carbon (OC)   performance of two linear multivariate and two machine learning methods for TN, OC and</t>
+          <t>Tomatoes are one of the most widely farmed and consumed vegetables in the world, and they are essential to the agricultural industry. Tomato plants are unfortunately prone to a number of illnesses, which can result in decreased production and quality and substantial financial losses. Grey leaf spot is one of the most prevalent diseases affecting tomato plants. It damages and destroys the leaves, which eventually prevents the plant from bearing fruit. Contact, invasion, latency, and onset are the four stages of the infection that the pathogen that causes grey leaf spot in tomato plants goes through. Early illness detection can provide effective management strategies and potentially avert widespread pandemics. Solanum lycopersicum, often known as the South Indian tomato, is a widely used vegetable in cooking. The tomato plant is widely cultivated and regarded as a significant agricultural commodity due to its ability to adapt to a range of environmental conditions and its abundance in potassium, vitamins C and K, and other minerals. However, growing tomatoes is not without its difficulties. Leaf diseases, which can reduce yields by as much as 60%, are one major challenge. The likelihood that conventional detection methods won't be able to keep up with the quick trends in plant diseases underscores the urgent need for creative alternatives. NNs provide a new technique for identifying tomato leaf disease. An inventive technique that utilizes and accurately diagnoses tomato leaf diseases is presented in this study. neural networks with convolutions.</t>
         </is>
       </c>
     </row>
     <row r="166">
       <c r="A166" t="inlineStr">
         <is>
-          <t>10.1016/j.ecoenv.2024.116867</t>
+          <t>10.1109/ICSC64553.2025.10968949</t>
         </is>
       </c>
       <c r="B166" t="inlineStr">
         <is>
-          <t>Application of machine learning approaches to predict ammonium nitrogen transport in different soil types and evaluate the contribution of control factors</t>
+          <t>Population Nutrition-Driven Crop Recommendations: Addressing Regional Micronutrient Deficiencies for Improved Public Health</t>
         </is>
       </c>
       <c r="C166" t="inlineStr">
         <is>
-          <t>['B Feng', 'J Ma', 'Y Liu', 'L Wang', 'X Zhang', 'Y Zhang']</t>
+          <t>P. Seshanth Vishal; P. Subedi; S. R. Divakarla; A. Harini; L. S</t>
         </is>
       </c>
       <c r="D166" t="n">
-        <v>2024</v>
+        <v>2025</v>
       </c>
       <c r="E166" t="inlineStr">
         <is>
-          <t>Ecotoxicology and …</t>
+          <t>2025 10th International Conference on Signal Processing and Communication (ICSC)</t>
         </is>
       </c>
       <c r="F166" t="n">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="G166" t="n">
-        <v>0.693429172039032</v>
+        <v>0.9080201387405396</v>
       </c>
       <c r="H166" t="inlineStr">
         <is>
-          <t>Tópico 1: model, nitrogen, network</t>
+          <t>Tópico 5: crop, soil, system</t>
         </is>
       </c>
       <c r="I166" t="inlineStr">
         <is>
-          <t>of nitrogen in soil damages the environment. Clarifying the mechanism of ammonium nitrogen  ( This study employed machine learning (ML) to identify the main influencing factors that</t>
+          <t>Crop yield optimization is paramount for an agriculture-based economy such as India, particularly in rural areas, which account for 92.02% of the agricultural workforce. However rural areas suffer the most from nutritional deficiencies. The proposed work attempts to combat the malnutrition by recommending crops which not only leverages the soil conditions (N, P, K, pH) and environmental conditions (humidity, rain, temperature) but also the micronutrient deficiencies among the regional population (Sodium, Potassium, Vitamin C, Calcium, Iron, Vitamin B6, Magnesium per 100mg). A hybrid dataset combining the crop recommendation dataset and USDA nutritional values dataset was prepared and utilized Six Machine Learning models-Decision trees, Support Vector machine (SVM), Logistic regression (LR), XGBoost, Random Forest (RF), and Naive Bayes (NB)-were trained and evaluated to determine the most effective model. The Random Forest classifier demonstrates an accuracy of 100% for the dataset used. The implementation of precision farming techniques optimizes crop yield production and contributes to food security and sustainable agriculture. Furthermore, the proposed work addresses the previously overlooked issue of deficiencies and recommends crops containing nutrients based on regional requirements. This approach will significantly impact agricultural produce and the holistic health of the population.</t>
         </is>
       </c>
     </row>
     <row r="167">
       <c r="A167" t="inlineStr">
         <is>
-          <t>10.1002/adfm.202413453</t>
+          <t>10.1109/CSDGAIS64098.2024.11064829</t>
         </is>
       </c>
       <c r="B167" t="inlineStr">
         <is>
-          <t>Machine Learning‐Assisted Design of Nitrogen‐Rich Covalent Triazine Frameworks Photocatalysts</t>
+          <t>Personalized Nutrition Recommendations Using Machine Learning</t>
         </is>
       </c>
       <c r="C167" t="inlineStr">
         <is>
-          <t>['M Wu', 'Z Song', 'Y Cui', 'Z Fu', 'K Hong', 'Q Li']</t>
+          <t>K. Samy; A. Osheba; H. S. El-Din; R. M. Sallam; M. A. Elaziz</t>
         </is>
       </c>
       <c r="D167" t="n">
-        <v>2025</v>
+        <v>2024</v>
       </c>
       <c r="E167" t="inlineStr">
         <is>
-          <t>Advanced Functional …</t>
+          <t>2024 International Conference on Smart-Digital-Green Technologies and Artificial Intelligence Sciences (CSDGAIS)</t>
         </is>
       </c>
       <c r="F167" t="n">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="G167" t="n">
-        <v>0.9573888778686523</v>
+        <v>0.9889057278633118</v>
       </c>
       <c r="H167" t="inlineStr">
         <is>
-          <t>Tópico 8: crop, soil, tomato</t>
+          <t>Tópico 5: crop, soil, system</t>
         </is>
       </c>
       <c r="I167" t="inlineStr">
         <is>
-          <t>To address this challenge, a machine-learning approach is developed to rationally design  nitrogen-rich  This work provides a new paradigm for machine learning to accelerate materials</t>
+          <t>Human nutrition is essential for maintaining health, promoting growth and development, preventing chronic diseases, managing medical conditions, and improving mental well-being. Nutritional imbalances, due to inadequate or excessive dietary intake, can lead to significant health issues. This project focuses on developing an advanced AI-based system to provide personalized nutrition recommendations for individuals with specific medical conditions. Utilizing sophisticated algorithms, the system analyzes a wide range of data, including health metrics, dietary preferences, and medical restrictions, to create customized diet plans that meet each user's unique needs. By leveraging AI technology, the system offers enhanced capabilities in food nutrition analysis, caloric intake calculation, and prediction of nutrient deficiencies or toxicities. It will address various conditions such as diabetes, hypertension, and food allergies, aligning diet plans with medical guidelines.</t>
         </is>
       </c>
     </row>
     <row r="168">
       <c r="A168" t="inlineStr">
         <is>
-          <t>10.1109/tasc.2022.3145290</t>
+          <t>10.1109/IGARSS.1990.688847</t>
         </is>
       </c>
       <c r="B168" t="inlineStr">
         <is>
-          <t>Study of liquid nitrogen insulation characteristics for superconducting transformers</t>
+          <t>Airborne Biochemical Mapping For Stress Detection In Coniferous Forests</t>
         </is>
       </c>
       <c r="C168" t="inlineStr">
         <is>
-          <t>['M Hu', 'QB Zhou', 'X Wang', 'FP Tang']</t>
+          <t>C. Banninger</t>
         </is>
       </c>
       <c r="D168" t="n">
-        <v>2022</v>
+        <v>1990</v>
       </c>
       <c r="E168" t="inlineStr">
         <is>
-          <t>IEEE Transactions …</t>
+          <t>10th Annual International Symposium on Geoscience and Remote Sensing</t>
         </is>
       </c>
       <c r="F168" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="G168" t="n">
-        <v>0.8471907377243042</v>
+        <v>0.5456134080886841</v>
       </c>
       <c r="H168" t="inlineStr">
         <is>
-          <t>Tópico 3: nitrogen, model, soil</t>
-        </is>
-      </c>
-      <c r="I168" t="inlineStr">
-        <is>
-          <t>nitrogen in real operation state is crucial. This paper firstly presents an AC withstand voltage  test of liquid nitrogen  insulation performance of liquid nitrogen is analyzed based on finite</t>
-        </is>
-      </c>
+          <t>Tópico 4: yolov, increase, map</t>
+        </is>
+      </c>
+      <c r="I168" t="inlineStr"/>
     </row>
     <row r="169">
       <c r="A169" t="inlineStr">
         <is>
-          <t>10.14569/ijacsa.2024.0150640</t>
+          <t>10.1109/IATMSI64286.2025.10985607</t>
         </is>
       </c>
       <c r="B169" t="inlineStr">
         <is>
-          <t>Foliar Nitrogen Estimation with Artificial Intelligence and Technological Tools: State of the Art and Future Challenges.</t>
+          <t>Proposed Convolutional Neural Network for the Detection of Guava Leaf Diseases</t>
         </is>
       </c>
       <c r="C169" t="inlineStr">
         <is>
-          <t>['Á Gallegos', 'ME Gavito']</t>
+          <t>R. Singh; S. Gupta; S. Aluvala; R. RiadHwsein; G. Sharma</t>
         </is>
       </c>
       <c r="D169" t="n">
-        <v>2024</v>
+        <v>2025</v>
       </c>
       <c r="E169" t="inlineStr">
         <is>
-          <t>International Journal of …</t>
+          <t>2025 IEEE International Conference on Interdisciplinary Approaches in Technology and Management for Social Innovation (IATMSI)</t>
         </is>
       </c>
       <c r="F169" t="n">
         <v>4</v>
       </c>
       <c r="G169" t="n">
-        <v>0.4387315213680267</v>
+        <v>0.7081536054611206</v>
       </c>
       <c r="H169" t="inlineStr">
         <is>
-          <t>Tópico 5: protein, approach, performance</t>
+          <t>Tópico 5: crop, soil, system</t>
         </is>
       </c>
       <c r="I169" t="inlineStr">
         <is>
-          <t>This review mainly focuses on nitrogen content, as color characteristics can conveniently  detect nitrogen deficiencies and excessive concentrations for adequate fertilization of crops.</t>
+          <t>Fruit cultivation is essential for domestic consumption and global trade, as agriculture continues to be a fundamental pillar of numerous economies worldwide. Guava (Psidium guajava) is a highly regarded fruit for its nutritional benefits, including high levels of dietary fiber, antioxidants, and vitamins A and C. Nevertheless, guava cultivation is encountering substantial obstacles due to various leaf diseases, which can harm the quality of the fruit and the yield. It is imperative to effectively manage these diseases to guarantee the optimal fruit production and guava crops' health. Timely and precise disease identification is critical to conventional disease management strategies, including applying fungicides, cultivating resistant varieties, and implementing cultural practices. Recent developments in deep learning, particularly Convolutional Neural Networks (CNNs), present promising solutions for the automated detection and classification of plant diseases based on visual symptoms. A CNN model that is specifically designed for the classification of guava leaf diseases, such as Canker, Dot, Mummification, Rust, and Healthy leaves, is proposed in this study. The model was trained on a comprehensive dataset that included 2108 training images and 527 testing images, and it was subsequently evaluated over a period of 30 epochs. It achieved an overall accuracy of 86.91%, with high precision, recall, and F1 scores across various disease categories. The model's potential for practical applications in agriculture, such as mobile apps or field-based systems, to assist farmers in the timely and effective management of diseases is evident in its robustness and reliability.</t>
         </is>
       </c>
     </row>
     <row r="170">
       <c r="A170" t="inlineStr">
         <is>
-          <t>10.1016/j.compag.2024.109341</t>
+          <t>10.1109/IATMSI64286.2025.10984798</t>
         </is>
       </c>
       <c r="B170" t="inlineStr">
         <is>
-          <t>Machine learning and fluorosensing for estimation of maize nitrogen status at early growth-stages</t>
+          <t>AI-enabled Recapitulated Neuro Fuzzy Optimization (RNFO)algorithm for evaluating the food consumption and nutrition during COVID-19</t>
         </is>
       </c>
       <c r="C170" t="inlineStr">
         <is>
-          <t>['D Mandal', 'R de Siqueira', 'L Longchamps']</t>
+          <t>H. M. Henrietta; A. Stanley Raj</t>
         </is>
       </c>
       <c r="D170" t="n">
-        <v>2024</v>
+        <v>2025</v>
       </c>
       <c r="E170" t="inlineStr">
         <is>
-          <t>… and Electronics in …</t>
+          <t>2025 IEEE International Conference on Interdisciplinary Approaches in Technology and Management for Social Innovation (IATMSI)</t>
         </is>
       </c>
       <c r="F170" t="n">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="G170" t="n">
-        <v>0.5827370285987854</v>
+        <v>0.5573188066482544</v>
       </c>
       <c r="H170" t="inlineStr">
         <is>
-          <t>Tópico 3: nitrogen, model, soil</t>
+          <t>Tópico 5: crop, soil, system</t>
         </is>
       </c>
       <c r="I170" t="inlineStr">
         <is>
-          <t>Hence, machine learning regression techniques are utilized in  assessing how well the  machine learning-trained model could  Subsequently, cross-site comparisons of nitrogen status</t>
+          <t>Food is essential for human survival and supports daily activities, energy production, and overall health. Adequate nutrient intake enables physiological and biochemical processes critical for energy conversion. Carbohydrates, among key nutrients, play a pivotal role in maintaining consistent energy levels. Malnutrition—marked by nutrient deficiencies or imbalances—is a pressing global health issue, with severe consequences for older adults who face age-related emotional and physical changes. Proper carbohydrate consumption helps regulate blood sugar and reduces the risk of chronic diseases. A balanced diet emphasizes natural foods while minimizing processed and high-fat animal products. This research explores the nutritional value of food, the impact of nutrient excess or deficiency, and carbohydrate’s health role. It employs an AI-driven Recapitulated Neuro-Fuzzy Optimization algorithm to analyze gender-based nutritional patterns during the COVID-19 pandemic.</t>
         </is>
       </c>
     </row>
     <row r="171">
       <c r="A171" t="inlineStr">
         <is>
-          <t>10.3390/rs16234514</t>
+          <t>10.1109/ECCE57851.2023.10101542</t>
         </is>
       </c>
       <c r="B171" t="inlineStr">
         <is>
-          <t>Recent Trends and Advances in Utilizing Digital Image Processing for Crop Nitrogen Management</t>
+          <t>An Efficient Transfer Learning-based Approach for Apple Leaf Disease Classification</t>
         </is>
       </c>
       <c r="C171" t="inlineStr">
         <is>
-          <t>['B Konara', 'M Krishnapillai', 'L Galagedara']</t>
+          <t>M. H. Ashmafee; T. Ahmed; S. Ahmed; M. B. Hasan; M. N. Jahan; A. B. M. Ashikur Rahman</t>
         </is>
       </c>
       <c r="D171" t="n">
-        <v>2024</v>
+        <v>2023</v>
       </c>
       <c r="E171" t="inlineStr">
         <is>
-          <t>Remote Sensing</t>
+          <t>2023 International Conference on Electrical, Computer and Communication Engineering (ECCE)</t>
         </is>
       </c>
       <c r="F171" t="n">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="G171" t="n">
-        <v>0.6484955549240112</v>
+        <v>0.554876446723938</v>
       </c>
       <c r="H171" t="inlineStr">
         <is>
-          <t>Tópico 3: nitrogen, model, soil</t>
+          <t>Tópico 5: crop, soil, system</t>
         </is>
       </c>
       <c r="I171" t="inlineStr">
         <is>
-          <t>Crop nitrogen (N) management in agricultural fields is crucial  Digital image processing (DIP)  offers a promising approach  Interest in integrating machine learning and deep learning</t>
+          <t>Correct identification and categorization of plant diseases are crucial for ensuring the safety of the global food supply and the overall financial success of stakeholders. In this regard, a wide range of solutions has been made available by in-troducing deep learning-based classification systems for different staple crops. Despite being one of the most important commercial crops in many parts of the globe, research proposing a smart solution for automatically classifying apple leaf diseases remains relatively unexplored. This work proposes a transfer learning-based approach for identifying apple leaf diseases. The system extracts features using a pretrained EfficientNetV2S architecture and passes to a classifier block for effective prediction. The class imbalance issues are tackled by utilizing runtime data augmentation. The effect of various hyperparameters, such as input resolution, learning rate, number of epochs, etc., has been investigated carefully. The competence of the proposed pipeline has been evaluated on the apple leaf disease subset from the publicly available ‘PlantVillage’ dataset, where it achieved an accuracy of 99.21 %, outperforming the existing works.</t>
         </is>
       </c>
     </row>
     <row r="172">
       <c r="A172" t="inlineStr">
         <is>
-          <t>10.1016/j.compag.2025.110366</t>
+          <t>10.1109/ICOSEC58147.2023.10276191</t>
         </is>
       </c>
       <c r="B172" t="inlineStr">
         <is>
-          <t>Integrating Feature Selection and Machine Learning for Nitrogen Assessment in Grapevine Leaves using In-Field Hyperspectral Imaging</t>
+          <t>Exploring a Novel Methodologies for Beetroot Leaf Disease Severity Prediction: Federated Learning and CNN</t>
         </is>
       </c>
       <c r="C172" t="inlineStr">
         <is>
-          <t>['AB Asad', 'A Paudel', 'S Kshetri', 'C Kang']</t>
+          <t>S. Mehta; V. Kukreja; V. Sharma; M. Manwal</t>
         </is>
       </c>
       <c r="D172" t="n">
-        <v>2025</v>
+        <v>2023</v>
       </c>
       <c r="E172" t="inlineStr">
         <is>
-          <t>arXiv preprint arXiv …</t>
+          <t>2023 4th International Conference on Smart Electronics and Communication (ICOSEC)</t>
         </is>
       </c>
       <c r="F172" t="n">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="G172" t="n">
-        <v>0.7452134490013123</v>
+        <v>0.5267233848571777</v>
       </c>
       <c r="H172" t="inlineStr">
         <is>
-          <t>Tópico 1: model, nitrogen, network</t>
+          <t>Tópico 5: crop, soil, system</t>
         </is>
       </c>
       <c r="I172" t="inlineStr">
         <is>
-          <t>Machine Learning (ML) models, Gradient Boosting and XGBoost, for predicting nitrogen   These findings indicated the robustness of these spectral regions for predicting nitrogen</t>
+          <t>This study explains how a federated learning Convolutional Neural Network (CNN) model is used to diagnose the various degrees of beetroot leaf diseases. Beetroot crops are essential to the world's food systems, but several illnesses often affect their quality and productivity. To suggest a CNN model using federated learning to analyse data from several clients while preserving privacy for a quick and precise diagnosis. The method analyses the severity of the five stages of beetroot leaf diseases using a federated learning technique across several local clients to use precision, recall, F1-score, and accuracy as performance measurements. The review showed that performance had improved consistently for all customers. As an example, Client X had a prediction accuracy of 0.97, which increased gradually to 0.98 for both Client P and Client R. Additionally, as shown by the macro-average (94.15-94.17%), weighted average (94.67%), and micro-average (94.62%) scores for top-performing customers, the model's performance remained stable and resilient throughout all severity levels. The study's findings support using a CNN model built on federated learning for scalable, effective, and privacy-preserving disease control in agriculture. The promising results suggest the potential for extending such approaches to other agricultural products, considerably advancing efforts to ensure global food security. The research also showed that the CNN model could learn and develop continuously in a federated learning scenario, highlighting its usefulness as a dynamic tool that adapts to new illness patterns. A paradigm shift in the approach to combating agricultural illnesses and increasing food supply is heralded by this study, which reveals a potential junction between machine learning and agricultural disease management. The findings motivate more research into the model's adaptability to other crops and pests, enhancing its contribution to resilient and sustainable farming systems.</t>
         </is>
       </c>
     </row>
     <row r="173">
       <c r="A173" t="inlineStr">
         <is>
-          <t>10.1016/j.compag.2025.110159</t>
+          <t>https://doi.org/10.1016/j.atech.2025.101406</t>
         </is>
       </c>
       <c r="B173" t="inlineStr">
         <is>
-          <t>Combining biomass production model with machine learning regression of critical nitrogen concentration for estimating grassland nitrogen requirements</t>
+          <t>A Review of the Application of UAV Multispectral Remote Sensing Technology in Precision Agriculture</t>
         </is>
       </c>
       <c r="C173" t="inlineStr">
         <is>
-          <t>['S Zhang', 'PE Lærke', 'MN Andersen']</t>
+          <t>Shuang Zhang; Xiaorui Wang; Hong Lin; Zhenping Qiang</t>
         </is>
       </c>
       <c r="D173" t="n">
@@ -7446,226 +7508,99 @@
       </c>
       <c r="E173" t="inlineStr">
         <is>
-          <t>… and Electronics in …</t>
+          <t>Smart Agricultural Technology</t>
         </is>
       </c>
       <c r="F173" t="n">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="G173" t="n">
-        <v>0.6437366008758545</v>
+        <v>0.7627755999565125</v>
       </c>
       <c r="H173" t="inlineStr">
         <is>
-          <t>Tópico 3: nitrogen, model, soil</t>
+          <t>Tópico 5: crop, soil, system</t>
         </is>
       </c>
       <c r="I173" t="inlineStr">
         <is>
-          <t>This paper presents a modelling ensemble to estimate nitrogen requirements (NR) for perennial  ryegrass and mixed grasslands from remotely sensed canopy reflectance. We designed</t>
+          <t>With the growing demand for precision agriculture, which requires high spatial and temporal resolution crop information, unmanned aerial vehicles (UAVs) equipped with multispectral sensors have become increasingly vital tools for agricultural management due to their real-time monitoring capabilities, flexibility, and cost-effectiveness. This paper provides a scoping review of advances in UAV-based multispectral remote sensing applications in precision agriculture, focusing on four key domains: crop growth monitoring, pest and disease identification, nutrient status assessment, and yield prediction. We offer a comprehensive analysis of the relevant literature, evaluating the principal challenges and opportunities associated with deploying this technology in the field. Our review indicates that traditional vegetation indices (e.g., NDVI, GNDVI, SAVI) have achieved mature application across diverse crops. In contrast, integrating emerging indices (e.g., TCARI, RDVI, OSAVI) with intelligent algorithms can significantly enhance monitoring accuracy and operational efficiency. In addition, we recommend that future research prioritize improvements in algorithmic precision, optimizing the data-processing workflows, and interdisciplinary collaboration to promote deeper integration of UAV-based multispectral sensing and artificial intelligence methods. Finally, we outline several practical research directions to inform and guide subsequent investigations.</t>
         </is>
       </c>
     </row>
     <row r="174">
       <c r="A174" t="inlineStr">
         <is>
-          <t>10.1016/j.ecz.2024.100006</t>
+          <t>https://doi.org/10.1017/S2040470019000013</t>
         </is>
       </c>
       <c r="B174" t="inlineStr">
         <is>
-          <t>Advancing agroecosystem modelling of nitrogen losses with machine learning</t>
+          <t>Proceedings of the British Society of Animal Science</t>
         </is>
       </c>
       <c r="C174" t="inlineStr">
         <is>
-          <t>['SK Lam', 'B Pan', 'AK Qin', 'D Chen']</t>
+          <t>Desconocido</t>
         </is>
       </c>
       <c r="D174" t="n">
-        <v>2024</v>
+        <v>2019</v>
       </c>
       <c r="E174" t="inlineStr">
         <is>
-          <t>Earth Critical Zone</t>
+          <t>Advances in Animal Biosciences</t>
         </is>
       </c>
       <c r="F174" t="n">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="G174" t="n">
-        <v>0.6710055470466614</v>
+        <v>0.8107492327690125</v>
       </c>
       <c r="H174" t="inlineStr">
         <is>
-          <t>Tópico 3: nitrogen, model, soil</t>
-        </is>
-      </c>
-      <c r="I174" t="inlineStr">
-        <is>
-          <t>Minimising nitrogen (N) losses from agricultural practices is critical to address the challenges  of environmental degradation and climate change, and safeguard global food production</t>
-        </is>
-      </c>
+          <t>Tópico 5: crop, soil, system</t>
+        </is>
+      </c>
+      <c r="I174" t="inlineStr"/>
     </row>
     <row r="175">
       <c r="A175" t="inlineStr">
         <is>
-          <t>10.3390/agriculture11080766</t>
+          <t>https://doi.org/10.1016/j.rineng.2025.104507</t>
         </is>
       </c>
       <c r="B175" t="inlineStr">
         <is>
-          <t>A computer-vision-based approach for nitrogen content estimation in plant leaves</t>
+          <t>The role of industry 4.0 technologies in the export flower industry: Insights from a systematic literature review and surveys in emerging economies</t>
         </is>
       </c>
       <c r="C175" t="inlineStr">
         <is>
-          <t>['T Haider', 'MS Farid', 'R Mahmood', 'A Ilyas', 'MH Khan']</t>
+          <t>Fernando Mantilla; Gonzalo Mejía; Diana Tascón</t>
         </is>
       </c>
       <c r="D175" t="n">
-        <v>2021</v>
+        <v>2025</v>
       </c>
       <c r="E175" t="inlineStr">
         <is>
-          <t>Agriculture</t>
+          <t>Results in Engineering</t>
         </is>
       </c>
       <c r="F175" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="G175" t="n">
-        <v>0.6479523181915283</v>
+        <v>0.5198959112167358</v>
       </c>
       <c r="H175" t="inlineStr">
         <is>
-          <t>Tópico 8: crop, soil, tomato</t>
+          <t>Tópico 7: model, data, study</t>
         </is>
       </c>
       <c r="I175" t="inlineStr">
-        <is>
-          <t>automated for years, and computer vision is proving to help  and apply different image  processing techniques to estimate the  of an image processing framework for nitrogen nutrient (n-</t>
-        </is>
-      </c>
-    </row>
-    <row r="176">
-      <c r="A176" t="inlineStr">
-        <is>
-          <t>10.3390/s22197338</t>
-        </is>
-      </c>
-      <c r="B176" t="inlineStr">
-        <is>
-          <t>A virtual sensing concept for nitrogen and phosphorus monitoring using machine learning techniques</t>
-        </is>
-      </c>
-      <c r="C176" t="inlineStr">
-        <is>
-          <t>['T Paepae', 'PN Bokoro', 'K Kyamakya']</t>
-        </is>
-      </c>
-      <c r="D176" t="n">
-        <v>2022</v>
-      </c>
-      <c r="E176" t="inlineStr">
-        <is>
-          <t>Sensors</t>
-        </is>
-      </c>
-      <c r="F176" t="n">
-        <v>0</v>
-      </c>
-      <c r="G176" t="n">
-        <v>0.7315318584442139</v>
-      </c>
-      <c r="H176" t="inlineStr">
-        <is>
-          <t>Tópico 1: model, nitrogen, network</t>
-        </is>
-      </c>
-      <c r="I176" t="inlineStr">
-        <is>
-          <t>of nitrogen (N) and phosphorus (P) in the water bodies. However, the high-frequency  monitoring of these water quality indicators is not economical. In these cases, machine learning</t>
-        </is>
-      </c>
-    </row>
-    <row r="177">
-      <c r="A177" t="inlineStr">
-        <is>
-          <t>https://doi.org/10.1016/j.atech.2025.101406</t>
-        </is>
-      </c>
-      <c r="B177" t="inlineStr">
-        <is>
-          <t>A Review of the Application of UAV Multispectral Remote Sensing Technology in Precision Agriculture</t>
-        </is>
-      </c>
-      <c r="C177" t="inlineStr">
-        <is>
-          <t>Shuang Zhang; Xiaorui Wang; Hong Lin; Zhenping Qiang</t>
-        </is>
-      </c>
-      <c r="D177" t="n">
-        <v>2025</v>
-      </c>
-      <c r="E177" t="inlineStr">
-        <is>
-          <t>Smart Agricultural Technology</t>
-        </is>
-      </c>
-      <c r="F177" t="n">
-        <v>0</v>
-      </c>
-      <c r="G177" t="n">
-        <v>0.4251807332038879</v>
-      </c>
-      <c r="H177" t="inlineStr">
-        <is>
-          <t>Tópico 1: model, nitrogen, network</t>
-        </is>
-      </c>
-      <c r="I177" t="inlineStr">
-        <is>
-          <t>With the growing demand for precision agriculture, which requires high spatial and temporal resolution crop information, unmanned aerial vehicles (UAVs) equipped with multispectral sensors have become increasingly vital tools for agricultural management due to their real-time monitoring capabilities, flexibility, and cost-effectiveness. This paper provides a scoping review of advances in UAV-based multispectral remote sensing applications in precision agriculture, focusing on four key domains: crop growth monitoring, pest and disease identification, nutrient status assessment, and yield prediction. We offer a comprehensive analysis of the relevant literature, evaluating the principal challenges and opportunities associated with deploying this technology in the field. Our review indicates that traditional vegetation indices (e.g., NDVI, GNDVI, SAVI) have achieved mature application across diverse crops. In contrast, integrating emerging indices (e.g., TCARI, RDVI, OSAVI) with intelligent algorithms can significantly enhance monitoring accuracy and operational efficiency. In addition, we recommend that future research prioritize improvements in algorithmic precision, optimizing the data-processing workflows, and interdisciplinary collaboration to promote deeper integration of UAV-based multispectral sensing and artificial intelligence methods. Finally, we outline several practical research directions to inform and guide subsequent investigations.</t>
-        </is>
-      </c>
-    </row>
-    <row r="178">
-      <c r="A178" t="inlineStr">
-        <is>
-          <t>https://doi.org/10.1016/j.rineng.2025.104507</t>
-        </is>
-      </c>
-      <c r="B178" t="inlineStr">
-        <is>
-          <t>The role of industry 4.0 technologies in the export flower industry: Insights from a systematic literature review and surveys in emerging economies</t>
-        </is>
-      </c>
-      <c r="C178" t="inlineStr">
-        <is>
-          <t>Fernando Mantilla; Gonzalo Mejía; Diana Tascón</t>
-        </is>
-      </c>
-      <c r="D178" t="n">
-        <v>2025</v>
-      </c>
-      <c r="E178" t="inlineStr">
-        <is>
-          <t>Results in Engineering</t>
-        </is>
-      </c>
-      <c r="F178" t="n">
-        <v>7</v>
-      </c>
-      <c r="G178" t="n">
-        <v>0.5375630259513855</v>
-      </c>
-      <c r="H178" t="inlineStr">
-        <is>
-          <t>Tópico 8: crop, soil, tomato</t>
-        </is>
-      </c>
-      <c r="I178" t="inlineStr">
         <is>
           <t>This paper aims to investigate the application of Industry 4.0 technologies in the flower industry focusing on the export business. The flower export sector is a very important industry for developing countries with considerable potential for improvement with Industry 4.0 technologies. Despite this potential, the deployment of these technologies encounters numerous barriers especially in emerging countries. This paper also studies the influence of these technologies on the productivity and sustainability of flower farms, including the entire process from planting to post-harvest management and distribution. We use a mixed-method strategy to accomplish these objectives: we performed a systematic literature review and carried out exploratory surveys administered to flower farmers in Ecuador and Colombia. The findings indicate that while the application of smart agricultural technologies in floriculture is currently restricted in emerging countries, there exists potential for its implementation. This research also points out obstacles for their adoption, including expenses, technical difficulties, and insufficient specialist. This research discusses the opportunities and problems associated with the integration of Industry 4.0 technologies in floriculture by offering both theoretical and practical insights, while also giving recommendations for industry stakeholders in managing this transition.</t>
         </is>

</xml_diff>

<commit_message>
se termina de hacer llenado con datos con apis
</commit_message>
<xml_diff>
--- a/referencias_con_topicos.xlsx
+++ b/referencias_con_topicos.xlsx
@@ -1362,7 +1362,7 @@
       </c>
       <c r="E23" t="inlineStr">
         <is>
-          <t>No especificado</t>
+          <t>2022 4th International Conference on Inventive Research in Computing Applications (ICIRCA)</t>
         </is>
       </c>
       <c r="F23" t="n">
@@ -2797,7 +2797,7 @@
       </c>
       <c r="E58" t="inlineStr">
         <is>
-          <t>No especificado</t>
+          <t>2022 13th International Conference on Computing Communication and Networking Technologies (ICCCNT)</t>
         </is>
       </c>
       <c r="F58" t="n">
@@ -2961,7 +2961,7 @@
       </c>
       <c r="E62" t="inlineStr">
         <is>
-          <t>No especificado</t>
+          <t>2022 IEEE 7th International conference for Convergence in Technology (I2CT)</t>
         </is>
       </c>
       <c r="F62" t="n">
@@ -4847,7 +4847,7 @@
       </c>
       <c r="E108" t="inlineStr">
         <is>
-          <t>No especificado</t>
+          <t>Proceedings of the AAAI Conference on Artificial Intelligence</t>
         </is>
       </c>
       <c r="F108" t="n">
@@ -5216,7 +5216,7 @@
       </c>
       <c r="E117" t="inlineStr">
         <is>
-          <t>No especificado</t>
+          <t>2022 2nd International Conference on Technological Advancements in Computational Sciences (ICTACS)</t>
         </is>
       </c>
       <c r="F117" t="n">
@@ -5257,7 +5257,7 @@
       </c>
       <c r="E118" t="inlineStr">
         <is>
-          <t>No especificado</t>
+          <t>2022 13th International Conference on Computing Communication and Networking Technologies (ICCCNT)</t>
         </is>
       </c>
       <c r="F118" t="n">
@@ -5339,7 +5339,7 @@
       </c>
       <c r="E120" t="inlineStr">
         <is>
-          <t>No especificado</t>
+          <t>2022 Fifth International Conference on Computational Intelligence and Communication Technologies (CCICT)</t>
         </is>
       </c>
       <c r="F120" t="n">
@@ -5503,7 +5503,7 @@
       </c>
       <c r="E124" t="inlineStr">
         <is>
-          <t>No especificado</t>
+          <t>2022 IEEE Delhi Section Conference (DELCON)</t>
         </is>
       </c>
       <c r="F124" t="n">
@@ -5585,7 +5585,7 @@
       </c>
       <c r="E126" t="inlineStr">
         <is>
-          <t>No especificado</t>
+          <t>2022 4th International Conference on Smart Systems and Inventive Technology (ICSSIT)</t>
         </is>
       </c>
       <c r="F126" t="n">
@@ -6610,7 +6610,7 @@
       </c>
       <c r="E151" t="inlineStr">
         <is>
-          <t>No especificado</t>
+          <t>Advances in parallel computing</t>
         </is>
       </c>
       <c r="F151" t="n">
@@ -6815,7 +6815,7 @@
       </c>
       <c r="E156" t="inlineStr">
         <is>
-          <t>No especificado</t>
+          <t>Springer eBooks</t>
         </is>
       </c>
       <c r="F156" t="n">

</xml_diff>